<commit_message>
Ajout de mes heures
</commit_message>
<xml_diff>
--- a/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire copy.xlsx
+++ b/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire copy.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alxbo\Source\Repos\mrjrdg\marque-sans-nom\Semainiers\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D18374-60D8-4B7C-B6EB-33884F24A293}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23136" windowHeight="12576" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -363,14 +357,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_)_ ;_ * \(#,##0.00\)_ ;_ * \-??_)_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="0\ %"/>
     <numFmt numFmtId="166" formatCode="[$-C0C]dd/mmm"/>
     <numFmt numFmtId="167" formatCode="\\;;;"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="24">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1495,35 +1489,56 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="19" fillId="9" borderId="8" xfId="8" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="12" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="16" xfId="9" applyBorder="1"/>
+    <xf numFmtId="167" fontId="23" fillId="11" borderId="20" xfId="9" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="20" xfId="8" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="5" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="37" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1541,69 +1556,48 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="19" fillId="9" borderId="8" xfId="8" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="12" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="16" xfId="9" applyBorder="1"/>
-    <xf numFmtId="167" fontId="23" fillId="11" borderId="20" xfId="9" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="20" xfId="8" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="8"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="5" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="37" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
-    <cellStyle name="Excel Built-in 60% - Accent4" xfId="7" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="Excel Built-in Bad" xfId="6" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Excel Built-in Good" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Excel Built-in Neutral" xfId="5" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Excel Built-in Normal" xfId="3" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Milliers" xfId="1" builtinId="3"/>
-    <cellStyle name="Neutre" xfId="9" builtinId="28"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Excel Built-in 60% - Accent4" xfId="7"/>
+    <cellStyle name="Excel Built-in Bad" xfId="6"/>
+    <cellStyle name="Excel Built-in Good" xfId="4"/>
+    <cellStyle name="Excel Built-in Neutral" xfId="5"/>
+    <cellStyle name="Excel Built-in Normal" xfId="3"/>
+    <cellStyle name="Good" xfId="8" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="9" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Satisfaisant" xfId="8" builtinId="26"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="42">
     <dxf>
@@ -2139,7 +2133,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2191,7 +2185,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2385,24 +2379,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AMK81"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10.44140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="74.109375" style="1" customWidth="1"/>
@@ -2426,23 +2420,23 @@
     <col min="29" max="1025" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="8" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="130" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="130"/>
+    <row r="1" spans="1:28" s="8" customFormat="1" ht="15.45" customHeight="1">
+      <c r="A1" s="160" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="160"/>
       <c r="C1" s="7"/>
-      <c r="D1" s="131" t="s">
+      <c r="D1" s="161" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
-      <c r="G1" s="131"/>
-      <c r="H1" s="131"/>
-      <c r="I1" s="131"/>
-      <c r="J1" s="131"/>
-      <c r="K1" s="131"/>
-      <c r="L1" s="131"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="161"/>
+      <c r="G1" s="161"/>
+      <c r="H1" s="161"/>
+      <c r="I1" s="161"/>
+      <c r="J1" s="161"/>
+      <c r="K1" s="161"/>
+      <c r="L1" s="161"/>
       <c r="N1" s="3"/>
       <c r="P1" s="9"/>
       <c r="Q1" s="8" t="s">
@@ -2453,21 +2447,21 @@
       <c r="Z1" s="3"/>
       <c r="AA1" s="10"/>
     </row>
-    <row r="2" spans="1:28" s="8" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="130" t="s">
+    <row r="2" spans="1:28" s="8" customFormat="1" ht="15.45" customHeight="1">
+      <c r="A2" s="160" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="130"/>
+      <c r="B2" s="160"/>
       <c r="C2" s="7"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
-      <c r="F2" s="130" t="s">
+      <c r="F2" s="160" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="130"/>
-      <c r="H2" s="130"/>
-      <c r="I2" s="130"/>
-      <c r="J2" s="130"/>
+      <c r="G2" s="160"/>
+      <c r="H2" s="160"/>
+      <c r="I2" s="160"/>
+      <c r="J2" s="160"/>
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
       <c r="N2" s="3"/>
@@ -2480,7 +2474,7 @@
       <c r="Z2" s="3"/>
       <c r="AA2" s="10"/>
     </row>
-    <row r="3" spans="1:28" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" s="8" customFormat="1" ht="15.6">
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -2498,7 +2492,7 @@
       <c r="Z3" s="3"/>
       <c r="AA3" s="10"/>
     </row>
-    <row r="4" spans="1:28" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" s="8" customFormat="1" ht="15.6">
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
@@ -2518,7 +2512,7 @@
       <c r="Z4" s="3"/>
       <c r="AA4" s="10"/>
     </row>
-    <row r="5" spans="1:28" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" s="8" customFormat="1" ht="15.6">
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
@@ -2542,7 +2536,7 @@
       </c>
       <c r="AA5" s="10"/>
     </row>
-    <row r="6" spans="1:28" s="8" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" s="8" customFormat="1" ht="16.2" customHeight="1">
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
@@ -2550,78 +2544,78 @@
       <c r="H6" s="3"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="132" t="s">
+      <c r="K6" s="152" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="132"/>
-      <c r="M6" s="132"/>
-      <c r="N6" s="132"/>
-      <c r="O6" s="132"/>
-      <c r="P6" s="132"/>
-      <c r="Q6" s="132"/>
-      <c r="R6" s="132"/>
-      <c r="S6" s="132" t="s">
+      <c r="L6" s="152"/>
+      <c r="M6" s="152"/>
+      <c r="N6" s="152"/>
+      <c r="O6" s="152"/>
+      <c r="P6" s="152"/>
+      <c r="Q6" s="152"/>
+      <c r="R6" s="152"/>
+      <c r="S6" s="152" t="s">
         <v>10</v>
       </c>
-      <c r="T6" s="132"/>
-      <c r="U6" s="132"/>
-      <c r="V6" s="132"/>
+      <c r="T6" s="152"/>
+      <c r="U6" s="152"/>
+      <c r="V6" s="152"/>
       <c r="Z6" s="17"/>
       <c r="AA6" s="10"/>
     </row>
-    <row r="7" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="133" t="s">
+    <row r="7" spans="1:28" ht="19.5" customHeight="1">
+      <c r="A7" s="153" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="134" t="s">
+      <c r="B7" s="154" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="135" t="s">
+      <c r="C7" s="155" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="135"/>
-      <c r="E7" s="135"/>
-      <c r="F7" s="135"/>
-      <c r="G7" s="136" t="s">
+      <c r="D7" s="155"/>
+      <c r="E7" s="155"/>
+      <c r="F7" s="155"/>
+      <c r="G7" s="156" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="137" t="s">
+      <c r="H7" s="157" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="138" t="s">
+      <c r="I7" s="158" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="138" t="s">
+      <c r="J7" s="158" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="139" t="s">
+      <c r="K7" s="159" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="139"/>
-      <c r="M7" s="139"/>
-      <c r="N7" s="139"/>
-      <c r="O7" s="139"/>
-      <c r="P7" s="139"/>
-      <c r="Q7" s="139"/>
-      <c r="R7" s="139"/>
-      <c r="S7" s="139"/>
-      <c r="T7" s="139"/>
-      <c r="U7" s="139"/>
-      <c r="V7" s="139"/>
-      <c r="W7" s="139"/>
-      <c r="X7" s="139"/>
-      <c r="Y7" s="139"/>
-      <c r="Z7" s="139"/>
-      <c r="AA7" s="143" t="s">
+      <c r="L7" s="159"/>
+      <c r="M7" s="159"/>
+      <c r="N7" s="159"/>
+      <c r="O7" s="159"/>
+      <c r="P7" s="159"/>
+      <c r="Q7" s="159"/>
+      <c r="R7" s="159"/>
+      <c r="S7" s="159"/>
+      <c r="T7" s="159"/>
+      <c r="U7" s="159"/>
+      <c r="V7" s="159"/>
+      <c r="W7" s="159"/>
+      <c r="X7" s="159"/>
+      <c r="Y7" s="159"/>
+      <c r="Z7" s="159"/>
+      <c r="AA7" s="149" t="s">
         <v>19</v>
       </c>
-      <c r="AB7" s="144" t="s">
+      <c r="AB7" s="150" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="133"/>
-      <c r="B8" s="134"/>
+    <row r="8" spans="1:28" ht="18.75" customHeight="1">
+      <c r="A8" s="153"/>
+      <c r="B8" s="154"/>
       <c r="C8" s="20" t="s">
         <v>21</v>
       </c>
@@ -2634,10 +2628,10 @@
       <c r="F8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="136"/>
-      <c r="H8" s="137"/>
-      <c r="I8" s="138"/>
-      <c r="J8" s="138"/>
+      <c r="G8" s="156"/>
+      <c r="H8" s="157"/>
+      <c r="I8" s="158"/>
+      <c r="J8" s="158"/>
       <c r="K8" s="21">
         <v>43838</v>
       </c>
@@ -2701,10 +2695,10 @@
         <f t="shared" si="0"/>
         <v>43943</v>
       </c>
-      <c r="AA8" s="143"/>
-      <c r="AB8" s="144"/>
-    </row>
-    <row r="9" spans="1:28" ht="18" x14ac:dyDescent="0.3">
+      <c r="AA8" s="149"/>
+      <c r="AB8" s="150"/>
+    </row>
+    <row r="9" spans="1:28" ht="18">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>25</v>
@@ -2736,7 +2730,7 @@
       <c r="AA9" s="33"/>
       <c r="AB9" s="34"/>
     </row>
-    <row r="10" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A10" s="35">
         <v>1</v>
       </c>
@@ -2791,7 +2785,7 @@
       </c>
       <c r="AB10" s="45"/>
     </row>
-    <row r="11" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A11" s="35">
         <v>2</v>
       </c>
@@ -2846,7 +2840,7 @@
       </c>
       <c r="AB11" s="48"/>
     </row>
-    <row r="12" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A12" s="35">
         <v>3</v>
       </c>
@@ -2900,7 +2894,7 @@
       </c>
       <c r="AB12" s="49"/>
     </row>
-    <row r="13" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A13" s="35">
         <v>4</v>
       </c>
@@ -2955,7 +2949,7 @@
       </c>
       <c r="AB13" s="48"/>
     </row>
-    <row r="14" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A14" s="35">
         <v>5</v>
       </c>
@@ -3010,7 +3004,7 @@
       </c>
       <c r="AB14" s="48"/>
     </row>
-    <row r="15" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A15" s="35">
         <v>6</v>
       </c>
@@ -3065,7 +3059,7 @@
       </c>
       <c r="AB15" s="48"/>
     </row>
-    <row r="16" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A16" s="35">
         <v>7</v>
       </c>
@@ -3120,7 +3114,7 @@
       </c>
       <c r="AB16" s="48"/>
     </row>
-    <row r="17" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A17" s="35">
         <v>8</v>
       </c>
@@ -3175,7 +3169,7 @@
       </c>
       <c r="AB17" s="48"/>
     </row>
-    <row r="18" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A18" s="35">
         <v>9</v>
       </c>
@@ -3230,7 +3224,7 @@
       </c>
       <c r="AB18" s="48"/>
     </row>
-    <row r="19" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A19" s="35">
         <v>10</v>
       </c>
@@ -3285,7 +3279,7 @@
       </c>
       <c r="AB19" s="48"/>
     </row>
-    <row r="20" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A20" s="35">
         <v>11</v>
       </c>
@@ -3340,7 +3334,7 @@
       </c>
       <c r="AB20" s="48"/>
     </row>
-    <row r="21" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" s="46" customFormat="1">
       <c r="A21" s="35">
         <v>12</v>
       </c>
@@ -3395,7 +3389,7 @@
       </c>
       <c r="AB21" s="48"/>
     </row>
-    <row r="22" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A22" s="35">
         <v>13</v>
       </c>
@@ -3450,7 +3444,7 @@
       </c>
       <c r="AB22" s="48"/>
     </row>
-    <row r="23" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A23" s="35">
         <v>14</v>
       </c>
@@ -3505,7 +3499,7 @@
       </c>
       <c r="AB23" s="48"/>
     </row>
-    <row r="24" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A24" s="35">
         <v>15</v>
       </c>
@@ -3560,7 +3554,7 @@
       </c>
       <c r="AB24" s="48"/>
     </row>
-    <row r="25" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A25" s="35">
         <v>16</v>
       </c>
@@ -3615,7 +3609,7 @@
       </c>
       <c r="AB25" s="48"/>
     </row>
-    <row r="26" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A26" s="35">
         <v>17</v>
       </c>
@@ -3670,7 +3664,7 @@
       </c>
       <c r="AB26" s="76"/>
     </row>
-    <row r="27" spans="1:28" s="79" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" s="79" customFormat="1" ht="15.6">
       <c r="A27" s="35">
         <v>18</v>
       </c>
@@ -3725,7 +3719,7 @@
       </c>
       <c r="AB27" s="48"/>
     </row>
-    <row r="28" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A28" s="35">
         <v>19</v>
       </c>
@@ -3780,7 +3774,7 @@
       </c>
       <c r="AB28" s="48"/>
     </row>
-    <row r="29" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A29" s="35">
         <v>20</v>
       </c>
@@ -3835,7 +3829,7 @@
       </c>
       <c r="AB29" s="48"/>
     </row>
-    <row r="30" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A30" s="35">
         <v>21</v>
       </c>
@@ -3890,7 +3884,7 @@
       </c>
       <c r="AB30" s="48"/>
     </row>
-    <row r="31" spans="1:28" s="79" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:28" s="79" customFormat="1" ht="15.6">
       <c r="A31" s="35">
         <v>22</v>
       </c>
@@ -3945,7 +3939,7 @@
       </c>
       <c r="AB31" s="48"/>
     </row>
-    <row r="32" spans="1:28" s="79" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:28" s="79" customFormat="1" ht="15.6">
       <c r="A32" s="35">
         <v>23</v>
       </c>
@@ -4000,7 +3994,7 @@
       </c>
       <c r="AB32" s="48"/>
     </row>
-    <row r="33" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A33" s="35">
         <v>24</v>
       </c>
@@ -4055,7 +4049,7 @@
       </c>
       <c r="AB33" s="48"/>
     </row>
-    <row r="34" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A34" s="35">
         <v>25</v>
       </c>
@@ -4110,7 +4104,7 @@
       </c>
       <c r="AB34" s="48"/>
     </row>
-    <row r="35" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A35" s="35">
         <v>27</v>
       </c>
@@ -4163,7 +4157,7 @@
       </c>
       <c r="AB35" s="48"/>
     </row>
-    <row r="36" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A36" s="35">
         <v>28</v>
       </c>
@@ -4216,7 +4210,7 @@
       </c>
       <c r="AB36" s="48"/>
     </row>
-    <row r="37" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A37" s="35">
         <v>29</v>
       </c>
@@ -4269,7 +4263,7 @@
       </c>
       <c r="AB37" s="48"/>
     </row>
-    <row r="38" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A38" s="35">
         <v>30</v>
       </c>
@@ -4322,7 +4316,7 @@
       </c>
       <c r="AB38" s="48"/>
     </row>
-    <row r="39" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A39" s="35">
         <v>31</v>
       </c>
@@ -4375,7 +4369,7 @@
       </c>
       <c r="AB39" s="48"/>
     </row>
-    <row r="40" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A40" s="35">
         <v>32</v>
       </c>
@@ -4428,7 +4422,7 @@
       </c>
       <c r="AB40" s="48"/>
     </row>
-    <row r="41" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A41" s="35">
         <v>33</v>
       </c>
@@ -4483,7 +4477,7 @@
       </c>
       <c r="AB41" s="48"/>
     </row>
-    <row r="42" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:28" s="46" customFormat="1">
       <c r="A42" s="35">
         <v>34</v>
       </c>
@@ -4536,7 +4530,7 @@
       </c>
       <c r="AB42" s="48"/>
     </row>
-    <row r="43" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A43" s="35">
         <v>35</v>
       </c>
@@ -4591,7 +4585,7 @@
       </c>
       <c r="AB43" s="48"/>
     </row>
-    <row r="44" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:28" s="46" customFormat="1">
       <c r="A44" s="35">
         <v>36</v>
       </c>
@@ -4646,7 +4640,7 @@
       </c>
       <c r="AB44" s="48"/>
     </row>
-    <row r="45" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A45" s="35">
         <v>37</v>
       </c>
@@ -4699,7 +4693,7 @@
       </c>
       <c r="AB45" s="48"/>
     </row>
-    <row r="46" spans="1:28" s="86" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:28" s="86" customFormat="1">
       <c r="A46" s="35">
         <v>39</v>
       </c>
@@ -4751,7 +4745,7 @@
       <c r="AA46" s="44"/>
       <c r="AB46" s="48"/>
     </row>
-    <row r="47" spans="1:28" s="86" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:28" s="86" customFormat="1" ht="15.6">
       <c r="A47" s="35">
         <v>40</v>
       </c>
@@ -4803,7 +4797,7 @@
       <c r="AA47" s="44"/>
       <c r="AB47" s="48"/>
     </row>
-    <row r="48" spans="1:28" s="46" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:28" s="46" customFormat="1" ht="18">
       <c r="A48" s="87"/>
       <c r="B48" s="24" t="s">
         <v>64</v>
@@ -4835,7 +4829,7 @@
       <c r="AA48" s="90"/>
       <c r="AB48" s="91"/>
     </row>
-    <row r="49" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A49" s="35">
         <v>1</v>
       </c>
@@ -4890,7 +4884,7 @@
       </c>
       <c r="AB49" s="48"/>
     </row>
-    <row r="50" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A50" s="35">
         <v>2</v>
       </c>
@@ -4943,7 +4937,7 @@
       </c>
       <c r="AB50" s="48"/>
     </row>
-    <row r="51" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A51" s="35">
         <v>3</v>
       </c>
@@ -4993,7 +4987,7 @@
       <c r="AA51" s="94"/>
       <c r="AB51" s="76"/>
     </row>
-    <row r="52" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A52" s="35">
         <v>4</v>
       </c>
@@ -5004,7 +4998,7 @@
         <v>3</v>
       </c>
       <c r="D52" s="37">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E52" s="37">
         <v>0</v>
@@ -5024,7 +5018,7 @@
       </c>
       <c r="J52" s="40">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="K52" s="42"/>
       <c r="L52" s="42"/>
@@ -5038,14 +5032,14 @@
       <c r="T52" s="68"/>
       <c r="U52" s="92"/>
       <c r="V52" s="122"/>
-      <c r="W52" s="73"/>
+      <c r="W52" s="53"/>
       <c r="X52" s="68"/>
       <c r="Y52" s="73"/>
       <c r="Z52" s="52"/>
       <c r="AA52" s="94"/>
       <c r="AB52" s="76"/>
     </row>
-    <row r="53" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A53" s="126">
         <v>5</v>
       </c>
@@ -5097,7 +5091,7 @@
       <c r="AA53" s="94"/>
       <c r="AB53" s="76"/>
     </row>
-    <row r="54" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A54" s="35">
         <v>6</v>
       </c>
@@ -5149,7 +5143,7 @@
       <c r="AA54" s="94"/>
       <c r="AB54" s="76"/>
     </row>
-    <row r="55" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A55" s="128">
         <v>7</v>
       </c>
@@ -5201,7 +5195,7 @@
       <c r="AA55" s="94"/>
       <c r="AB55" s="76"/>
     </row>
-    <row r="56" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A56" s="35">
         <v>8</v>
       </c>
@@ -5253,7 +5247,7 @@
       <c r="AA56" s="94"/>
       <c r="AB56" s="76"/>
     </row>
-    <row r="57" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A57" s="35">
         <v>9</v>
       </c>
@@ -5305,11 +5299,11 @@
       <c r="AA57" s="94"/>
       <c r="AB57" s="76"/>
     </row>
-    <row r="58" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A58" s="35">
         <v>10</v>
       </c>
-      <c r="B58" s="152" t="s">
+      <c r="B58" s="136" t="s">
         <v>82</v>
       </c>
       <c r="C58" s="37">
@@ -5350,18 +5344,18 @@
       <c r="T58" s="73"/>
       <c r="U58" s="73"/>
       <c r="V58" s="52"/>
-      <c r="W58" s="148"/>
-      <c r="X58" s="149"/>
+      <c r="W58" s="132"/>
+      <c r="X58" s="133"/>
       <c r="Y58" s="73"/>
       <c r="Z58" s="52"/>
       <c r="AA58" s="94"/>
       <c r="AB58" s="76"/>
     </row>
-    <row r="59" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A59" s="35">
         <v>11</v>
       </c>
-      <c r="B59" s="152" t="s">
+      <c r="B59" s="136" t="s">
         <v>83</v>
       </c>
       <c r="C59" s="37">
@@ -5402,18 +5396,18 @@
       <c r="T59" s="73"/>
       <c r="U59" s="73"/>
       <c r="V59" s="52"/>
-      <c r="W59" s="151"/>
+      <c r="W59" s="135"/>
       <c r="X59" s="124"/>
       <c r="Y59" s="73"/>
       <c r="Z59" s="52"/>
       <c r="AA59" s="94"/>
       <c r="AB59" s="76"/>
     </row>
-    <row r="60" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A60" s="35">
         <v>12</v>
       </c>
-      <c r="B60" s="152" t="s">
+      <c r="B60" s="136" t="s">
         <v>77</v>
       </c>
       <c r="C60" s="37">
@@ -5454,27 +5448,27 @@
       <c r="T60" s="73"/>
       <c r="U60" s="73"/>
       <c r="V60" s="52"/>
-      <c r="W60" s="150"/>
+      <c r="W60" s="134"/>
       <c r="X60" s="124"/>
       <c r="Y60" s="73"/>
       <c r="Z60" s="52"/>
       <c r="AA60" s="94"/>
       <c r="AB60" s="76"/>
     </row>
-    <row r="61" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A61" s="35">
         <v>13</v>
       </c>
-      <c r="B61" s="152" t="s">
+      <c r="B61" s="136" t="s">
         <v>84</v>
       </c>
-      <c r="C61" s="147">
-        <v>0</v>
-      </c>
-      <c r="D61" s="147">
-        <v>0</v>
-      </c>
-      <c r="E61" s="147">
+      <c r="C61" s="131">
+        <v>0</v>
+      </c>
+      <c r="D61" s="131">
+        <v>0</v>
+      </c>
+      <c r="E61" s="131">
         <v>0.25</v>
       </c>
       <c r="F61" s="37">
@@ -5513,11 +5507,11 @@
       <c r="AA61" s="94"/>
       <c r="AB61" s="76"/>
     </row>
-    <row r="62" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A62" s="35">
         <v>14</v>
       </c>
-      <c r="B62" s="152" t="s">
+      <c r="B62" s="136" t="s">
         <v>85</v>
       </c>
       <c r="C62" s="37">
@@ -5565,7 +5559,7 @@
       <c r="AA62" s="94"/>
       <c r="AB62" s="76"/>
     </row>
-    <row r="63" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A63" s="35">
         <v>15</v>
       </c>
@@ -5617,7 +5611,7 @@
       <c r="AA63" s="94"/>
       <c r="AB63" s="76"/>
     </row>
-    <row r="64" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A64" s="35">
         <v>16</v>
       </c>
@@ -5669,7 +5663,7 @@
       <c r="AA64" s="94"/>
       <c r="AB64" s="76"/>
     </row>
-    <row r="65" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A65" s="35"/>
       <c r="B65" s="69"/>
       <c r="C65" s="37"/>
@@ -5699,7 +5693,7 @@
       <c r="AA65" s="94"/>
       <c r="AB65" s="76"/>
     </row>
-    <row r="66" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A66" s="35"/>
       <c r="B66" s="69"/>
       <c r="C66" s="37"/>
@@ -5729,7 +5723,7 @@
       <c r="AA66" s="94"/>
       <c r="AB66" s="76"/>
     </row>
-    <row r="67" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A67" s="35"/>
       <c r="B67" s="69"/>
       <c r="C67" s="37"/>
@@ -5759,7 +5753,7 @@
       <c r="AA67" s="94"/>
       <c r="AB67" s="76"/>
     </row>
-    <row r="68" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A68" s="35"/>
       <c r="B68" s="69"/>
       <c r="C68" s="37"/>
@@ -5789,17 +5783,17 @@
       <c r="AA68" s="94"/>
       <c r="AB68" s="76"/>
     </row>
-    <row r="69" spans="1:28" s="46" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="156"/>
-      <c r="B69" s="157"/>
-      <c r="C69" s="158"/>
-      <c r="D69" s="158"/>
-      <c r="E69" s="158"/>
-      <c r="F69" s="158"/>
-      <c r="G69" s="159"/>
-      <c r="H69" s="160"/>
-      <c r="I69" s="161"/>
-      <c r="J69" s="161"/>
+    <row r="69" spans="1:28" s="46" customFormat="1" ht="16.2" thickBot="1">
+      <c r="A69" s="140"/>
+      <c r="B69" s="141"/>
+      <c r="C69" s="142"/>
+      <c r="D69" s="142"/>
+      <c r="E69" s="142"/>
+      <c r="F69" s="142"/>
+      <c r="G69" s="143"/>
+      <c r="H69" s="144"/>
+      <c r="I69" s="145"/>
+      <c r="J69" s="145"/>
       <c r="K69" s="95"/>
       <c r="L69" s="95"/>
       <c r="M69" s="95"/>
@@ -5807,30 +5801,30 @@
       <c r="O69" s="95"/>
       <c r="P69" s="95"/>
       <c r="Q69" s="95"/>
-      <c r="R69" s="155"/>
+      <c r="R69" s="139"/>
       <c r="S69" s="95"/>
       <c r="T69" s="95"/>
       <c r="U69" s="95"/>
       <c r="V69" s="96"/>
       <c r="W69" s="95"/>
-      <c r="X69" s="146"/>
+      <c r="X69" s="130"/>
       <c r="Y69" s="95"/>
       <c r="Z69" s="96"/>
       <c r="AA69" s="97"/>
       <c r="AB69" s="98"/>
     </row>
-    <row r="70" spans="1:28" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="145" t="s">
+    <row r="70" spans="1:28" ht="16.5" customHeight="1" thickBot="1">
+      <c r="A70" s="151" t="s">
         <v>68</v>
       </c>
-      <c r="B70" s="145"/>
+      <c r="B70" s="151"/>
       <c r="C70" s="99">
         <f>SUM(C10:C69)</f>
         <v>109.5</v>
       </c>
       <c r="D70" s="99">
         <f>SUM(D10:D69)</f>
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E70" s="99">
         <f>SUM(E10:E69)</f>
@@ -5844,8 +5838,8 @@
       <c r="H70" s="99"/>
       <c r="I70" s="101"/>
       <c r="J70" s="99">
-        <f t="shared" si="3"/>
-        <v>392.25</v>
+        <f>SUM(C70:F70)</f>
+        <v>396.25</v>
       </c>
       <c r="K70" s="102"/>
       <c r="L70" s="102"/>
@@ -5863,24 +5857,24 @@
       <c r="X70" s="102"/>
       <c r="Y70" s="102"/>
       <c r="Z70" s="102"/>
-      <c r="AA70" s="153">
+      <c r="AA70" s="137">
         <f>SUM(AA10:AA69)</f>
         <v>0.25</v>
       </c>
-      <c r="AB70" s="154"/>
-    </row>
-    <row r="71" spans="1:28" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="140" t="s">
+      <c r="AB70" s="138"/>
+    </row>
+    <row r="71" spans="1:28" ht="16.95" customHeight="1" thickBot="1">
+      <c r="A71" s="146" t="s">
         <v>69</v>
       </c>
-      <c r="B71" s="140"/>
+      <c r="B71" s="146"/>
       <c r="C71" s="99">
         <f>135-C70</f>
         <v>25.5</v>
       </c>
       <c r="D71" s="99">
         <f>135-D70</f>
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E71" s="99">
         <f>135-E70</f>
@@ -5894,8 +5888,8 @@
       <c r="H71" s="99"/>
       <c r="I71" s="99"/>
       <c r="J71" s="99">
-        <f t="shared" si="3"/>
-        <v>147.75</v>
+        <f>SUM(C71:F71)</f>
+        <v>143.75</v>
       </c>
       <c r="K71" s="102"/>
       <c r="L71" s="102"/>
@@ -5916,11 +5910,11 @@
       <c r="AA71" s="102"/>
       <c r="AB71" s="102"/>
     </row>
-    <row r="72" spans="1:28" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="141" t="s">
+    <row r="72" spans="1:28" ht="16.95" customHeight="1">
+      <c r="A72" s="147" t="s">
         <v>70</v>
       </c>
-      <c r="B72" s="141"/>
+      <c r="B72" s="147"/>
       <c r="C72" s="99"/>
       <c r="D72" s="99"/>
       <c r="E72" s="99"/>
@@ -5951,11 +5945,11 @@
       <c r="AA72" s="102"/>
       <c r="AB72" s="102"/>
     </row>
-    <row r="73" spans="1:28" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="140" t="s">
+    <row r="73" spans="1:28" ht="16.95" customHeight="1">
+      <c r="A73" s="146" t="s">
         <v>71</v>
       </c>
-      <c r="B73" s="140"/>
+      <c r="B73" s="146"/>
       <c r="C73" s="99"/>
       <c r="D73" s="99"/>
       <c r="E73" s="103"/>
@@ -5968,7 +5962,7 @@
       </c>
       <c r="J73" s="99">
         <f>SUM(J10:J69)</f>
-        <v>392.25</v>
+        <v>396.25</v>
       </c>
       <c r="K73" s="102"/>
       <c r="L73" s="102"/>
@@ -5989,7 +5983,7 @@
       <c r="AA73" s="102"/>
       <c r="AB73" s="102"/>
     </row>
-    <row r="74" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:28" ht="15.6">
       <c r="A74" s="105"/>
       <c r="B74" s="105"/>
       <c r="C74" s="106"/>
@@ -6019,11 +6013,11 @@
       <c r="AA74" s="102"/>
       <c r="AB74" s="102"/>
     </row>
-    <row r="75" spans="1:28" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="141" t="s">
+    <row r="75" spans="1:28" ht="16.2" customHeight="1">
+      <c r="A75" s="147" t="s">
         <v>72</v>
       </c>
-      <c r="B75" s="141"/>
+      <c r="B75" s="147"/>
       <c r="C75" s="99">
         <f>135*4</f>
         <v>540</v>
@@ -6054,14 +6048,14 @@
       <c r="AA75" s="102"/>
       <c r="AB75" s="102"/>
     </row>
-    <row r="76" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="142" t="s">
+    <row r="76" spans="1:28" ht="15.6">
+      <c r="A76" s="148" t="s">
         <v>73</v>
       </c>
-      <c r="B76" s="142"/>
+      <c r="B76" s="148"/>
       <c r="C76" s="99">
         <f>C75-J73</f>
-        <v>147.75</v>
+        <v>143.75</v>
       </c>
       <c r="D76" s="106"/>
       <c r="E76" s="106"/>
@@ -6089,7 +6083,7 @@
       <c r="AA76" s="102"/>
       <c r="AB76" s="102"/>
     </row>
-    <row r="77" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:28" ht="15.6">
       <c r="A77" s="107"/>
       <c r="B77" s="105"/>
       <c r="C77" s="108"/>
@@ -6102,12 +6096,12 @@
       <c r="J77" s="110"/>
       <c r="AA77" s="102"/>
     </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:28">
       <c r="D78" s="111"/>
       <c r="E78" s="111"/>
       <c r="F78" s="111"/>
     </row>
-    <row r="79" spans="1:28" s="113" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:28" s="113" customFormat="1" ht="13.8">
       <c r="A79" s="112"/>
       <c r="C79" s="114"/>
       <c r="D79" s="114"/>
@@ -6122,7 +6116,7 @@
       <c r="Z79" s="117"/>
       <c r="AA79" s="118"/>
     </row>
-    <row r="80" spans="1:28" s="113" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:28" s="113" customFormat="1" ht="13.8">
       <c r="C80" s="114"/>
       <c r="D80" s="114"/>
       <c r="E80" s="114"/>
@@ -6136,7 +6130,7 @@
       <c r="Z80" s="117"/>
       <c r="AA80" s="118"/>
     </row>
-    <row r="81" spans="3:27" s="113" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="3:27" s="113" customFormat="1" ht="13.8">
       <c r="C81" s="114"/>
       <c r="D81" s="114"/>
       <c r="E81" s="114"/>
@@ -6152,14 +6146,11 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K6:R6"/>
     <mergeCell ref="S6:V6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
@@ -6169,11 +6160,14 @@
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="K7:Z7"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
   </mergeCells>
   <conditionalFormatting sqref="H19">
     <cfRule type="containsText" dxfId="41" priority="19" operator="containsText" text="En cours">
@@ -6338,7 +6332,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H9:H69" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H9:H69">
       <formula1>"En attente,En cours,Terminé"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6350,19 +6344,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMK3"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1025" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="119" t="s">
         <v>6</v>
       </c>
@@ -6370,7 +6364,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -6378,7 +6372,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -6393,12 +6387,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMK1"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1025" width="10.6640625" style="1"/>
   </cols>

</xml_diff>

<commit_message>
Rapport de sprint 2
</commit_message>
<xml_diff>
--- a/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire copy.xlsx
+++ b/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire copy.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alxbo\Source\Repos\mrjrdg\marque-sans-nom\Semainiers\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B40382-F080-4DEA-B9D8-2FC2EE8A7683}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23136" windowHeight="12576" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="87">
   <si>
     <t>UQÀM - Hiver 2020</t>
   </si>
@@ -333,9 +339,6 @@
     <t>Correctifs et modifications sur la supression d'entreprise et rejoindre evenement</t>
   </si>
   <si>
-    <t>Babillards de commentaires - Repousser au 3 ieme Sprint</t>
-  </si>
-  <si>
     <t>Pages gestion d'evenement (Create,Edit,Delete) - Edit et Delete repousser 3ieme Sprint</t>
   </si>
   <si>
@@ -352,19 +355,25 @@
   </si>
   <si>
     <t>Améliorer le visuel (business-create, business-list, business-edit)</t>
+  </si>
+  <si>
+    <t>Rédaction du rapport de sprint 2</t>
+  </si>
+  <si>
+    <t>Améliorer le visuel (messagerie) - REPOUSSÉ AU SPRINT 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_)_ ;_ * \(#,##0.00\)_ ;_ * \-??_)_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="0\ %"/>
     <numFmt numFmtId="166" formatCode="[$-C0C]dd/mmm"/>
     <numFmt numFmtId="167" formatCode="\\;;;"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -512,30 +521,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFC00000"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -597,12 +591,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFAAAC4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
@@ -610,6 +598,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -1091,7 +1084,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -1101,9 +1094,10 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1473,32 +1467,12 @@
     <xf numFmtId="0" fontId="19" fillId="9" borderId="16" xfId="8" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="19" fillId="9" borderId="8" xfId="8" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="12" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="1" fillId="11" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="16" xfId="9" applyBorder="1"/>
-    <xf numFmtId="167" fontId="23" fillId="11" borderId="20" xfId="9" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="16" xfId="9" applyBorder="1"/>
+    <xf numFmtId="167" fontId="20" fillId="10" borderId="20" xfId="9" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1540,6 +1514,36 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1556,50 +1560,104 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="19" fillId="0" borderId="20" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="19" fillId="0" borderId="8" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="15" xfId="10" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="22" xfId="10" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="10">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Excel Built-in 60% - Accent4" xfId="7"/>
-    <cellStyle name="Excel Built-in Bad" xfId="6"/>
-    <cellStyle name="Excel Built-in Good" xfId="4"/>
-    <cellStyle name="Excel Built-in Neutral" xfId="5"/>
-    <cellStyle name="Excel Built-in Normal" xfId="3"/>
-    <cellStyle name="Good" xfId="8" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="9" builtinId="28"/>
+  <cellStyles count="11">
+    <cellStyle name="Excel Built-in 60% - Accent4" xfId="7" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Excel Built-in Bad" xfId="6" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Excel Built-in Good" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Excel Built-in Neutral" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Excel Built-in Normal" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Insatisfaisant" xfId="10" builtinId="27"/>
+    <cellStyle name="Milliers" xfId="1" builtinId="3"/>
+    <cellStyle name="Neutre" xfId="9" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Satisfaisant" xfId="8" builtinId="26"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="45">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1791,43 +1849,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2379,24 +2400,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AMK81"/>
+  <dimension ref="A1:AMK80"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.44140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="74.109375" style="1" customWidth="1"/>
@@ -2420,23 +2441,23 @@
     <col min="29" max="1025" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="8" customFormat="1" ht="15.45" customHeight="1">
-      <c r="A1" s="160" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="160"/>
+    <row r="1" spans="1:28" s="8" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="141"/>
       <c r="C1" s="7"/>
-      <c r="D1" s="161" t="s">
+      <c r="D1" s="142" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="161"/>
-      <c r="F1" s="161"/>
-      <c r="G1" s="161"/>
-      <c r="H1" s="161"/>
-      <c r="I1" s="161"/>
-      <c r="J1" s="161"/>
-      <c r="K1" s="161"/>
-      <c r="L1" s="161"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="142"/>
+      <c r="J1" s="142"/>
+      <c r="K1" s="142"/>
+      <c r="L1" s="142"/>
       <c r="N1" s="3"/>
       <c r="P1" s="9"/>
       <c r="Q1" s="8" t="s">
@@ -2447,21 +2468,21 @@
       <c r="Z1" s="3"/>
       <c r="AA1" s="10"/>
     </row>
-    <row r="2" spans="1:28" s="8" customFormat="1" ht="15.45" customHeight="1">
-      <c r="A2" s="160" t="s">
+    <row r="2" spans="1:28" s="8" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="141" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="160"/>
+      <c r="B2" s="141"/>
       <c r="C2" s="7"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
-      <c r="F2" s="160" t="s">
+      <c r="F2" s="141" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="160"/>
-      <c r="H2" s="160"/>
-      <c r="I2" s="160"/>
-      <c r="J2" s="160"/>
+      <c r="G2" s="141"/>
+      <c r="H2" s="141"/>
+      <c r="I2" s="141"/>
+      <c r="J2" s="141"/>
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
       <c r="N2" s="3"/>
@@ -2474,7 +2495,7 @@
       <c r="Z2" s="3"/>
       <c r="AA2" s="10"/>
     </row>
-    <row r="3" spans="1:28" s="8" customFormat="1" ht="15.6">
+    <row r="3" spans="1:28" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -2492,7 +2513,7 @@
       <c r="Z3" s="3"/>
       <c r="AA3" s="10"/>
     </row>
-    <row r="4" spans="1:28" s="8" customFormat="1" ht="15.6">
+    <row r="4" spans="1:28" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
@@ -2512,7 +2533,7 @@
       <c r="Z4" s="3"/>
       <c r="AA4" s="10"/>
     </row>
-    <row r="5" spans="1:28" s="8" customFormat="1" ht="15.6">
+    <row r="5" spans="1:28" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
@@ -2536,7 +2557,7 @@
       </c>
       <c r="AA5" s="10"/>
     </row>
-    <row r="6" spans="1:28" s="8" customFormat="1" ht="16.2" customHeight="1">
+    <row r="6" spans="1:28" s="8" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
@@ -2544,78 +2565,78 @@
       <c r="H6" s="3"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="152" t="s">
+      <c r="K6" s="143" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="152"/>
-      <c r="M6" s="152"/>
-      <c r="N6" s="152"/>
-      <c r="O6" s="152"/>
-      <c r="P6" s="152"/>
-      <c r="Q6" s="152"/>
-      <c r="R6" s="152"/>
-      <c r="S6" s="152" t="s">
+      <c r="L6" s="143"/>
+      <c r="M6" s="143"/>
+      <c r="N6" s="143"/>
+      <c r="O6" s="143"/>
+      <c r="P6" s="143"/>
+      <c r="Q6" s="143"/>
+      <c r="R6" s="143"/>
+      <c r="S6" s="143" t="s">
         <v>10</v>
       </c>
-      <c r="T6" s="152"/>
-      <c r="U6" s="152"/>
-      <c r="V6" s="152"/>
+      <c r="T6" s="143"/>
+      <c r="U6" s="143"/>
+      <c r="V6" s="143"/>
       <c r="Z6" s="17"/>
       <c r="AA6" s="10"/>
     </row>
-    <row r="7" spans="1:28" ht="19.5" customHeight="1">
-      <c r="A7" s="153" t="s">
+    <row r="7" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="144" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="154" t="s">
+      <c r="B7" s="145" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="155" t="s">
+      <c r="C7" s="146" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="155"/>
-      <c r="E7" s="155"/>
-      <c r="F7" s="155"/>
-      <c r="G7" s="156" t="s">
+      <c r="D7" s="146"/>
+      <c r="E7" s="146"/>
+      <c r="F7" s="146"/>
+      <c r="G7" s="147" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="157" t="s">
+      <c r="H7" s="148" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="158" t="s">
+      <c r="I7" s="149" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="158" t="s">
+      <c r="J7" s="149" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="159" t="s">
+      <c r="K7" s="150" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="159"/>
-      <c r="M7" s="159"/>
-      <c r="N7" s="159"/>
-      <c r="O7" s="159"/>
-      <c r="P7" s="159"/>
-      <c r="Q7" s="159"/>
-      <c r="R7" s="159"/>
-      <c r="S7" s="159"/>
-      <c r="T7" s="159"/>
-      <c r="U7" s="159"/>
-      <c r="V7" s="159"/>
-      <c r="W7" s="159"/>
-      <c r="X7" s="159"/>
-      <c r="Y7" s="159"/>
-      <c r="Z7" s="159"/>
-      <c r="AA7" s="149" t="s">
+      <c r="L7" s="150"/>
+      <c r="M7" s="150"/>
+      <c r="N7" s="150"/>
+      <c r="O7" s="150"/>
+      <c r="P7" s="150"/>
+      <c r="Q7" s="150"/>
+      <c r="R7" s="150"/>
+      <c r="S7" s="150"/>
+      <c r="T7" s="150"/>
+      <c r="U7" s="150"/>
+      <c r="V7" s="150"/>
+      <c r="W7" s="150"/>
+      <c r="X7" s="150"/>
+      <c r="Y7" s="150"/>
+      <c r="Z7" s="150"/>
+      <c r="AA7" s="154" t="s">
         <v>19</v>
       </c>
-      <c r="AB7" s="150" t="s">
+      <c r="AB7" s="155" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="18.75" customHeight="1">
-      <c r="A8" s="153"/>
-      <c r="B8" s="154"/>
+    <row r="8" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="144"/>
+      <c r="B8" s="145"/>
       <c r="C8" s="20" t="s">
         <v>21</v>
       </c>
@@ -2628,10 +2649,10 @@
       <c r="F8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="156"/>
-      <c r="H8" s="157"/>
-      <c r="I8" s="158"/>
-      <c r="J8" s="158"/>
+      <c r="G8" s="147"/>
+      <c r="H8" s="148"/>
+      <c r="I8" s="149"/>
+      <c r="J8" s="149"/>
       <c r="K8" s="21">
         <v>43838</v>
       </c>
@@ -2695,10 +2716,10 @@
         <f t="shared" si="0"/>
         <v>43943</v>
       </c>
-      <c r="AA8" s="149"/>
-      <c r="AB8" s="150"/>
-    </row>
-    <row r="9" spans="1:28" ht="18">
+      <c r="AA8" s="154"/>
+      <c r="AB8" s="155"/>
+    </row>
+    <row r="9" spans="1:28" ht="18" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>25</v>
@@ -2730,7 +2751,7 @@
       <c r="AA9" s="33"/>
       <c r="AB9" s="34"/>
     </row>
-    <row r="10" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="10" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="35">
         <v>1</v>
       </c>
@@ -2785,7 +2806,7 @@
       </c>
       <c r="AB10" s="45"/>
     </row>
-    <row r="11" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="11" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="35">
         <v>2</v>
       </c>
@@ -2840,7 +2861,7 @@
       </c>
       <c r="AB11" s="48"/>
     </row>
-    <row r="12" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="12" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="35">
         <v>3</v>
       </c>
@@ -2894,7 +2915,7 @@
       </c>
       <c r="AB12" s="49"/>
     </row>
-    <row r="13" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="13" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="35">
         <v>4</v>
       </c>
@@ -2949,7 +2970,7 @@
       </c>
       <c r="AB13" s="48"/>
     </row>
-    <row r="14" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="14" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="35">
         <v>5</v>
       </c>
@@ -3004,7 +3025,7 @@
       </c>
       <c r="AB14" s="48"/>
     </row>
-    <row r="15" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="15" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="35">
         <v>6</v>
       </c>
@@ -3059,7 +3080,7 @@
       </c>
       <c r="AB15" s="48"/>
     </row>
-    <row r="16" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="16" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="35">
         <v>7</v>
       </c>
@@ -3114,7 +3135,7 @@
       </c>
       <c r="AB16" s="48"/>
     </row>
-    <row r="17" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="17" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="35">
         <v>8</v>
       </c>
@@ -3169,7 +3190,7 @@
       </c>
       <c r="AB17" s="48"/>
     </row>
-    <row r="18" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="18" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="35">
         <v>9</v>
       </c>
@@ -3224,7 +3245,7 @@
       </c>
       <c r="AB18" s="48"/>
     </row>
-    <row r="19" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="19" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="35">
         <v>10</v>
       </c>
@@ -3279,7 +3300,7 @@
       </c>
       <c r="AB19" s="48"/>
     </row>
-    <row r="20" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="20" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="35">
         <v>11</v>
       </c>
@@ -3334,7 +3355,7 @@
       </c>
       <c r="AB20" s="48"/>
     </row>
-    <row r="21" spans="1:28" s="46" customFormat="1">
+    <row r="21" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="35">
         <v>12</v>
       </c>
@@ -3389,7 +3410,7 @@
       </c>
       <c r="AB21" s="48"/>
     </row>
-    <row r="22" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="22" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="35">
         <v>13</v>
       </c>
@@ -3444,7 +3465,7 @@
       </c>
       <c r="AB22" s="48"/>
     </row>
-    <row r="23" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="23" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="35">
         <v>14</v>
       </c>
@@ -3499,7 +3520,7 @@
       </c>
       <c r="AB23" s="48"/>
     </row>
-    <row r="24" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="24" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="35">
         <v>15</v>
       </c>
@@ -3554,7 +3575,7 @@
       </c>
       <c r="AB24" s="48"/>
     </row>
-    <row r="25" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="25" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="35">
         <v>16</v>
       </c>
@@ -3609,7 +3630,7 @@
       </c>
       <c r="AB25" s="48"/>
     </row>
-    <row r="26" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="26" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="35">
         <v>17</v>
       </c>
@@ -3664,7 +3685,7 @@
       </c>
       <c r="AB26" s="76"/>
     </row>
-    <row r="27" spans="1:28" s="79" customFormat="1" ht="15.6">
+    <row r="27" spans="1:28" s="79" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="35">
         <v>18</v>
       </c>
@@ -3719,7 +3740,7 @@
       </c>
       <c r="AB27" s="48"/>
     </row>
-    <row r="28" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="28" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="35">
         <v>19</v>
       </c>
@@ -3774,7 +3795,7 @@
       </c>
       <c r="AB28" s="48"/>
     </row>
-    <row r="29" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="29" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="35">
         <v>20</v>
       </c>
@@ -3829,7 +3850,7 @@
       </c>
       <c r="AB29" s="48"/>
     </row>
-    <row r="30" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="30" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="35">
         <v>21</v>
       </c>
@@ -3884,7 +3905,7 @@
       </c>
       <c r="AB30" s="48"/>
     </row>
-    <row r="31" spans="1:28" s="79" customFormat="1" ht="15.6">
+    <row r="31" spans="1:28" s="79" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="35">
         <v>22</v>
       </c>
@@ -3939,7 +3960,7 @@
       </c>
       <c r="AB31" s="48"/>
     </row>
-    <row r="32" spans="1:28" s="79" customFormat="1" ht="15.6">
+    <row r="32" spans="1:28" s="79" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="35">
         <v>23</v>
       </c>
@@ -3994,7 +4015,7 @@
       </c>
       <c r="AB32" s="48"/>
     </row>
-    <row r="33" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="33" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="35">
         <v>24</v>
       </c>
@@ -4049,7 +4070,7 @@
       </c>
       <c r="AB33" s="48"/>
     </row>
-    <row r="34" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="34" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="35">
         <v>25</v>
       </c>
@@ -4104,7 +4125,7 @@
       </c>
       <c r="AB34" s="48"/>
     </row>
-    <row r="35" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="35" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="35">
         <v>27</v>
       </c>
@@ -4157,7 +4178,7 @@
       </c>
       <c r="AB35" s="48"/>
     </row>
-    <row r="36" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="36" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="35">
         <v>28</v>
       </c>
@@ -4210,7 +4231,7 @@
       </c>
       <c r="AB36" s="48"/>
     </row>
-    <row r="37" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="37" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="35">
         <v>29</v>
       </c>
@@ -4263,7 +4284,7 @@
       </c>
       <c r="AB37" s="48"/>
     </row>
-    <row r="38" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="38" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="35">
         <v>30</v>
       </c>
@@ -4316,7 +4337,7 @@
       </c>
       <c r="AB38" s="48"/>
     </row>
-    <row r="39" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="39" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="35">
         <v>31</v>
       </c>
@@ -4369,7 +4390,7 @@
       </c>
       <c r="AB39" s="48"/>
     </row>
-    <row r="40" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="40" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="35">
         <v>32</v>
       </c>
@@ -4422,7 +4443,7 @@
       </c>
       <c r="AB40" s="48"/>
     </row>
-    <row r="41" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="41" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="35">
         <v>33</v>
       </c>
@@ -4477,7 +4498,7 @@
       </c>
       <c r="AB41" s="48"/>
     </row>
-    <row r="42" spans="1:28" s="46" customFormat="1">
+    <row r="42" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="35">
         <v>34</v>
       </c>
@@ -4530,7 +4551,7 @@
       </c>
       <c r="AB42" s="48"/>
     </row>
-    <row r="43" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="43" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="35">
         <v>35</v>
       </c>
@@ -4585,7 +4606,7 @@
       </c>
       <c r="AB43" s="48"/>
     </row>
-    <row r="44" spans="1:28" s="46" customFormat="1">
+    <row r="44" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="35">
         <v>36</v>
       </c>
@@ -4640,7 +4661,7 @@
       </c>
       <c r="AB44" s="48"/>
     </row>
-    <row r="45" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="45" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="35">
         <v>37</v>
       </c>
@@ -4693,7 +4714,7 @@
       </c>
       <c r="AB45" s="48"/>
     </row>
-    <row r="46" spans="1:28" s="86" customFormat="1">
+    <row r="46" spans="1:28" s="86" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="35">
         <v>39</v>
       </c>
@@ -4745,7 +4766,7 @@
       <c r="AA46" s="44"/>
       <c r="AB46" s="48"/>
     </row>
-    <row r="47" spans="1:28" s="86" customFormat="1" ht="15.6">
+    <row r="47" spans="1:28" s="86" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="35">
         <v>40</v>
       </c>
@@ -4797,7 +4818,7 @@
       <c r="AA47" s="44"/>
       <c r="AB47" s="48"/>
     </row>
-    <row r="48" spans="1:28" s="46" customFormat="1" ht="18">
+    <row r="48" spans="1:28" s="46" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A48" s="87"/>
       <c r="B48" s="24" t="s">
         <v>64</v>
@@ -4829,7 +4850,7 @@
       <c r="AA48" s="90"/>
       <c r="AB48" s="91"/>
     </row>
-    <row r="49" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="49" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="35">
         <v>1</v>
       </c>
@@ -4859,7 +4880,7 @@
         <v>7</v>
       </c>
       <c r="J49" s="40">
-        <f t="shared" ref="J49:J71" si="3">SUM(C49:F49)</f>
+        <f t="shared" ref="J49:J62" si="3">SUM(C49:F49)</f>
         <v>8.75</v>
       </c>
       <c r="K49" s="73"/>
@@ -4884,7 +4905,7 @@
       </c>
       <c r="AB49" s="48"/>
     </row>
-    <row r="50" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="50" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="35">
         <v>2</v>
       </c>
@@ -4937,7 +4958,7 @@
       </c>
       <c r="AB50" s="48"/>
     </row>
-    <row r="51" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="51" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="35">
         <v>3</v>
       </c>
@@ -4987,7 +5008,7 @@
       <c r="AA51" s="94"/>
       <c r="AB51" s="76"/>
     </row>
-    <row r="52" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="52" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="35">
         <v>4</v>
       </c>
@@ -5039,12 +5060,12 @@
       <c r="AA52" s="94"/>
       <c r="AB52" s="76"/>
     </row>
-    <row r="53" spans="1:28" s="46" customFormat="1" ht="15.6">
-      <c r="A53" s="126">
+    <row r="53" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="159">
         <v>5</v>
       </c>
-      <c r="B53" s="127" t="s">
-        <v>80</v>
+      <c r="B53" s="160" t="s">
+        <v>79</v>
       </c>
       <c r="C53" s="37">
         <v>8</v>
@@ -5091,7 +5112,7 @@
       <c r="AA53" s="94"/>
       <c r="AB53" s="76"/>
     </row>
-    <row r="54" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="54" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="35">
         <v>6</v>
       </c>
@@ -5143,15 +5164,15 @@
       <c r="AA54" s="94"/>
       <c r="AB54" s="76"/>
     </row>
-    <row r="55" spans="1:28" s="46" customFormat="1" ht="15.6">
-      <c r="A55" s="128">
+    <row r="55" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="35">
         <v>7</v>
       </c>
-      <c r="B55" s="129" t="s">
-        <v>79</v>
+      <c r="B55" s="69" t="s">
+        <v>76</v>
       </c>
       <c r="C55" s="37">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D55" s="37">
         <v>0</v>
@@ -5164,17 +5185,17 @@
       </c>
       <c r="G55" s="71">
         <f>VLOOKUP(H55,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="H55" s="39" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I55" s="40">
         <v>8</v>
       </c>
       <c r="J55" s="40">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K55" s="42"/>
       <c r="L55" s="42"/>
@@ -5185,25 +5206,25 @@
       <c r="Q55" s="73"/>
       <c r="R55" s="93"/>
       <c r="S55" s="73"/>
-      <c r="T55" s="42"/>
-      <c r="U55" s="92"/>
-      <c r="V55" s="122"/>
+      <c r="T55" s="73"/>
+      <c r="U55" s="73"/>
+      <c r="V55" s="52"/>
       <c r="W55" s="73"/>
-      <c r="X55" s="68"/>
+      <c r="X55" s="73"/>
       <c r="Y55" s="73"/>
       <c r="Z55" s="52"/>
       <c r="AA55" s="94"/>
       <c r="AB55" s="76"/>
     </row>
-    <row r="56" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="56" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="35">
         <v>8</v>
       </c>
       <c r="B56" s="69" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C56" s="37">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D56" s="37">
         <v>0</v>
@@ -5212,7 +5233,7 @@
         <v>0</v>
       </c>
       <c r="F56" s="37">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G56" s="71">
         <f>VLOOKUP(H56,Feuil2!$A$1:$B$3,2,0)</f>
@@ -5226,7 +5247,7 @@
       </c>
       <c r="J56" s="40">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K56" s="42"/>
       <c r="L56" s="42"/>
@@ -5239,7 +5260,7 @@
       <c r="S56" s="73"/>
       <c r="T56" s="73"/>
       <c r="U56" s="73"/>
-      <c r="V56" s="52"/>
+      <c r="V56" s="123"/>
       <c r="W56" s="73"/>
       <c r="X56" s="73"/>
       <c r="Y56" s="73"/>
@@ -5247,12 +5268,12 @@
       <c r="AA56" s="94"/>
       <c r="AB56" s="76"/>
     </row>
-    <row r="57" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="57" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="35">
         <v>9</v>
       </c>
-      <c r="B57" s="69" t="s">
-        <v>75</v>
+      <c r="B57" s="131" t="s">
+        <v>81</v>
       </c>
       <c r="C57" s="37">
         <v>0</v>
@@ -5261,24 +5282,24 @@
         <v>0</v>
       </c>
       <c r="E57" s="37">
-        <v>0</v>
+        <v>11.5</v>
       </c>
       <c r="F57" s="37">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G57" s="71">
         <f>VLOOKUP(H57,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H57" s="39" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I57" s="40">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J57" s="40">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>11.5</v>
       </c>
       <c r="K57" s="42"/>
       <c r="L57" s="42"/>
@@ -5291,19 +5312,19 @@
       <c r="S57" s="73"/>
       <c r="T57" s="73"/>
       <c r="U57" s="73"/>
-      <c r="V57" s="123"/>
-      <c r="W57" s="73"/>
-      <c r="X57" s="73"/>
+      <c r="V57" s="52"/>
+      <c r="W57" s="127"/>
+      <c r="X57" s="128"/>
       <c r="Y57" s="73"/>
       <c r="Z57" s="52"/>
       <c r="AA57" s="94"/>
       <c r="AB57" s="76"/>
     </row>
-    <row r="58" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="58" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="35">
         <v>10</v>
       </c>
-      <c r="B58" s="136" t="s">
+      <c r="B58" s="131" t="s">
         <v>82</v>
       </c>
       <c r="C58" s="37">
@@ -5313,24 +5334,24 @@
         <v>0</v>
       </c>
       <c r="E58" s="37">
-        <v>11.5</v>
+        <v>0.75</v>
       </c>
       <c r="F58" s="37">
         <v>0</v>
       </c>
       <c r="G58" s="71">
         <f>VLOOKUP(H58,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H58" s="39" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I58" s="40">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="J58" s="40">
         <f t="shared" si="3"/>
-        <v>11.5</v>
+        <v>0.75</v>
       </c>
       <c r="K58" s="42"/>
       <c r="L58" s="42"/>
@@ -5344,19 +5365,19 @@
       <c r="T58" s="73"/>
       <c r="U58" s="73"/>
       <c r="V58" s="52"/>
-      <c r="W58" s="132"/>
-      <c r="X58" s="133"/>
+      <c r="W58" s="130"/>
+      <c r="X58" s="124"/>
       <c r="Y58" s="73"/>
       <c r="Z58" s="52"/>
       <c r="AA58" s="94"/>
       <c r="AB58" s="76"/>
     </row>
-    <row r="59" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="59" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="35">
         <v>11</v>
       </c>
-      <c r="B59" s="136" t="s">
-        <v>83</v>
+      <c r="B59" s="131" t="s">
+        <v>77</v>
       </c>
       <c r="C59" s="37">
         <v>0</v>
@@ -5365,7 +5386,7 @@
         <v>0</v>
       </c>
       <c r="E59" s="37">
-        <v>0.75</v>
+        <v>4</v>
       </c>
       <c r="F59" s="37">
         <v>0</v>
@@ -5378,11 +5399,11 @@
         <v>2</v>
       </c>
       <c r="I59" s="40">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J59" s="40">
         <f t="shared" si="3"/>
-        <v>0.75</v>
+        <v>4</v>
       </c>
       <c r="K59" s="42"/>
       <c r="L59" s="42"/>
@@ -5396,28 +5417,28 @@
       <c r="T59" s="73"/>
       <c r="U59" s="73"/>
       <c r="V59" s="52"/>
-      <c r="W59" s="135"/>
+      <c r="W59" s="129"/>
       <c r="X59" s="124"/>
       <c r="Y59" s="73"/>
       <c r="Z59" s="52"/>
       <c r="AA59" s="94"/>
       <c r="AB59" s="76"/>
     </row>
-    <row r="60" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="60" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="35">
         <v>12</v>
       </c>
-      <c r="B60" s="136" t="s">
-        <v>77</v>
-      </c>
-      <c r="C60" s="37">
-        <v>0</v>
-      </c>
-      <c r="D60" s="37">
-        <v>0</v>
-      </c>
-      <c r="E60" s="37">
-        <v>4</v>
+      <c r="B60" s="131" t="s">
+        <v>83</v>
+      </c>
+      <c r="C60" s="126">
+        <v>0</v>
+      </c>
+      <c r="D60" s="126">
+        <v>0</v>
+      </c>
+      <c r="E60" s="126">
+        <v>0.25</v>
       </c>
       <c r="F60" s="37">
         <v>0</v>
@@ -5430,11 +5451,11 @@
         <v>2</v>
       </c>
       <c r="I60" s="40">
-        <v>3</v>
+        <v>0.25</v>
       </c>
       <c r="J60" s="40">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>0.25</v>
       </c>
       <c r="K60" s="42"/>
       <c r="L60" s="42"/>
@@ -5448,28 +5469,28 @@
       <c r="T60" s="73"/>
       <c r="U60" s="73"/>
       <c r="V60" s="52"/>
-      <c r="W60" s="134"/>
+      <c r="W60" s="124"/>
       <c r="X60" s="124"/>
       <c r="Y60" s="73"/>
       <c r="Z60" s="52"/>
       <c r="AA60" s="94"/>
       <c r="AB60" s="76"/>
     </row>
-    <row r="61" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="61" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="35">
         <v>13</v>
       </c>
-      <c r="B61" s="136" t="s">
+      <c r="B61" s="131" t="s">
         <v>84</v>
       </c>
-      <c r="C61" s="131">
-        <v>0</v>
-      </c>
-      <c r="D61" s="131">
-        <v>0</v>
-      </c>
-      <c r="E61" s="131">
-        <v>0.25</v>
+      <c r="C61" s="37">
+        <v>0</v>
+      </c>
+      <c r="D61" s="37">
+        <v>0</v>
+      </c>
+      <c r="E61" s="37">
+        <v>2.5</v>
       </c>
       <c r="F61" s="37">
         <v>0</v>
@@ -5482,11 +5503,11 @@
         <v>2</v>
       </c>
       <c r="I61" s="40">
-        <v>0.25</v>
+        <v>3</v>
       </c>
       <c r="J61" s="40">
         <f t="shared" si="3"/>
-        <v>0.25</v>
+        <v>2.5</v>
       </c>
       <c r="K61" s="42"/>
       <c r="L61" s="42"/>
@@ -5507,21 +5528,21 @@
       <c r="AA61" s="94"/>
       <c r="AB61" s="76"/>
     </row>
-    <row r="62" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="62" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="35">
         <v>14</v>
       </c>
-      <c r="B62" s="136" t="s">
-        <v>85</v>
+      <c r="B62" s="69" t="s">
+        <v>78</v>
       </c>
       <c r="C62" s="37">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D62" s="37">
         <v>0</v>
       </c>
       <c r="E62" s="37">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="F62" s="37">
         <v>0</v>
@@ -5534,11 +5555,11 @@
         <v>2</v>
       </c>
       <c r="I62" s="40">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J62" s="40">
         <f t="shared" si="3"/>
-        <v>2.5</v>
+        <v>8</v>
       </c>
       <c r="K62" s="42"/>
       <c r="L62" s="42"/>
@@ -5552,22 +5573,22 @@
       <c r="T62" s="73"/>
       <c r="U62" s="73"/>
       <c r="V62" s="52"/>
-      <c r="W62" s="124"/>
+      <c r="W62" s="73"/>
       <c r="X62" s="124"/>
       <c r="Y62" s="73"/>
       <c r="Z62" s="52"/>
       <c r="AA62" s="94"/>
       <c r="AB62" s="76"/>
     </row>
-    <row r="63" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="63" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="35">
         <v>15</v>
       </c>
       <c r="B63" s="69" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C63" s="37">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D63" s="37">
         <v>0</v>
@@ -5576,7 +5597,7 @@
         <v>0</v>
       </c>
       <c r="F63" s="37">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G63" s="71">
         <f>VLOOKUP(H63,Feuil2!$A$1:$B$3,2,0)</f>
@@ -5586,11 +5607,11 @@
         <v>2</v>
       </c>
       <c r="I63" s="40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J63" s="40">
-        <f t="shared" si="3"/>
-        <v>8</v>
+        <f t="shared" ref="J63:J64" si="4">SUM(C63:F63)</f>
+        <v>7</v>
       </c>
       <c r="K63" s="42"/>
       <c r="L63" s="42"/>
@@ -5611,15 +5632,15 @@
       <c r="AA63" s="94"/>
       <c r="AB63" s="76"/>
     </row>
-    <row r="64" spans="1:28" s="46" customFormat="1" ht="15.6">
-      <c r="A64" s="35">
-        <v>16</v>
-      </c>
-      <c r="B64" s="69" t="s">
-        <v>81</v>
+    <row r="64" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="159">
+        <v>17</v>
+      </c>
+      <c r="B64" s="160" t="s">
+        <v>86</v>
       </c>
       <c r="C64" s="37">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D64" s="37">
         <v>0</v>
@@ -5628,24 +5649,19 @@
         <v>0</v>
       </c>
       <c r="F64" s="37">
+        <v>0</v>
+      </c>
+      <c r="G64" s="71"/>
+      <c r="H64" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="G64" s="71">
-        <f>VLOOKUP(H64,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H64" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="I64" s="40">
-        <v>1</v>
-      </c>
+      <c r="I64" s="40"/>
       <c r="J64" s="40">
-        <f t="shared" ref="J64" si="4">SUM(C64:F64)</f>
-        <v>7</v>
-      </c>
-      <c r="K64" s="42"/>
-      <c r="L64" s="42"/>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K64" s="73"/>
+      <c r="L64" s="73"/>
       <c r="M64" s="73"/>
       <c r="N64" s="52"/>
       <c r="O64" s="73"/>
@@ -5657,23 +5673,42 @@
       <c r="U64" s="73"/>
       <c r="V64" s="52"/>
       <c r="W64" s="73"/>
-      <c r="X64" s="124"/>
+      <c r="X64" s="128"/>
       <c r="Y64" s="73"/>
       <c r="Z64" s="52"/>
       <c r="AA64" s="94"/>
       <c r="AB64" s="76"/>
     </row>
-    <row r="65" spans="1:28" s="46" customFormat="1" ht="15.6">
-      <c r="A65" s="35"/>
-      <c r="B65" s="69"/>
-      <c r="C65" s="37"/>
-      <c r="D65" s="37"/>
-      <c r="E65" s="37"/>
-      <c r="F65" s="37"/>
+    <row r="65" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="35">
+        <v>18</v>
+      </c>
+      <c r="B65" s="69" t="s">
+        <v>85</v>
+      </c>
+      <c r="C65" s="37">
+        <v>0</v>
+      </c>
+      <c r="D65" s="37">
+        <v>0</v>
+      </c>
+      <c r="E65" s="37">
+        <v>1.5</v>
+      </c>
+      <c r="F65" s="37">
+        <v>0</v>
+      </c>
       <c r="G65" s="71"/>
-      <c r="H65" s="39"/>
-      <c r="I65" s="40"/>
-      <c r="J65" s="40"/>
+      <c r="H65" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="I65" s="40">
+        <v>3</v>
+      </c>
+      <c r="J65" s="40">
+        <f t="shared" ref="J65" si="5">SUM(C65:F65)</f>
+        <v>1.5</v>
+      </c>
       <c r="K65" s="73"/>
       <c r="L65" s="73"/>
       <c r="M65" s="73"/>
@@ -5687,13 +5722,13 @@
       <c r="U65" s="73"/>
       <c r="V65" s="52"/>
       <c r="W65" s="73"/>
-      <c r="X65" s="124"/>
+      <c r="X65" s="128"/>
       <c r="Y65" s="73"/>
       <c r="Z65" s="52"/>
       <c r="AA65" s="94"/>
       <c r="AB65" s="76"/>
     </row>
-    <row r="66" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="66" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="35"/>
       <c r="B66" s="69"/>
       <c r="C66" s="37"/>
@@ -5717,13 +5752,13 @@
       <c r="U66" s="73"/>
       <c r="V66" s="52"/>
       <c r="W66" s="73"/>
-      <c r="X66" s="124"/>
+      <c r="X66" s="157"/>
       <c r="Y66" s="73"/>
       <c r="Z66" s="52"/>
       <c r="AA66" s="94"/>
       <c r="AB66" s="76"/>
     </row>
-    <row r="67" spans="1:28" s="46" customFormat="1" ht="15.6">
+    <row r="67" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="35"/>
       <c r="B67" s="69"/>
       <c r="C67" s="37"/>
@@ -5747,99 +5782,119 @@
       <c r="U67" s="73"/>
       <c r="V67" s="52"/>
       <c r="W67" s="73"/>
-      <c r="X67" s="124"/>
+      <c r="X67" s="157"/>
       <c r="Y67" s="73"/>
       <c r="Z67" s="52"/>
       <c r="AA67" s="94"/>
       <c r="AB67" s="76"/>
     </row>
-    <row r="68" spans="1:28" s="46" customFormat="1" ht="15.6">
-      <c r="A68" s="35"/>
-      <c r="B68" s="69"/>
-      <c r="C68" s="37"/>
-      <c r="D68" s="37"/>
-      <c r="E68" s="37"/>
-      <c r="F68" s="37"/>
-      <c r="G68" s="71"/>
-      <c r="H68" s="39"/>
-      <c r="I68" s="40"/>
-      <c r="J68" s="40"/>
-      <c r="K68" s="73"/>
-      <c r="L68" s="73"/>
-      <c r="M68" s="73"/>
-      <c r="N68" s="52"/>
-      <c r="O68" s="73"/>
-      <c r="P68" s="73"/>
-      <c r="Q68" s="73"/>
-      <c r="R68" s="93"/>
-      <c r="S68" s="73"/>
-      <c r="T68" s="73"/>
-      <c r="U68" s="73"/>
-      <c r="V68" s="52"/>
-      <c r="W68" s="73"/>
-      <c r="X68" s="124"/>
-      <c r="Y68" s="73"/>
-      <c r="Z68" s="52"/>
-      <c r="AA68" s="94"/>
-      <c r="AB68" s="76"/>
-    </row>
-    <row r="69" spans="1:28" s="46" customFormat="1" ht="16.2" thickBot="1">
-      <c r="A69" s="140"/>
-      <c r="B69" s="141"/>
-      <c r="C69" s="142"/>
-      <c r="D69" s="142"/>
-      <c r="E69" s="142"/>
-      <c r="F69" s="142"/>
-      <c r="G69" s="143"/>
-      <c r="H69" s="144"/>
-      <c r="I69" s="145"/>
-      <c r="J69" s="145"/>
-      <c r="K69" s="95"/>
-      <c r="L69" s="95"/>
-      <c r="M69" s="95"/>
-      <c r="N69" s="96"/>
-      <c r="O69" s="95"/>
-      <c r="P69" s="95"/>
-      <c r="Q69" s="95"/>
-      <c r="R69" s="139"/>
-      <c r="S69" s="95"/>
-      <c r="T69" s="95"/>
-      <c r="U69" s="95"/>
-      <c r="V69" s="96"/>
-      <c r="W69" s="95"/>
-      <c r="X69" s="130"/>
-      <c r="Y69" s="95"/>
-      <c r="Z69" s="96"/>
-      <c r="AA69" s="97"/>
-      <c r="AB69" s="98"/>
-    </row>
-    <row r="70" spans="1:28" ht="16.5" customHeight="1" thickBot="1">
+    <row r="68" spans="1:28" s="46" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="135"/>
+      <c r="B68" s="136"/>
+      <c r="C68" s="137"/>
+      <c r="D68" s="137"/>
+      <c r="E68" s="137"/>
+      <c r="F68" s="137"/>
+      <c r="G68" s="138"/>
+      <c r="H68" s="139"/>
+      <c r="I68" s="140"/>
+      <c r="J68" s="140"/>
+      <c r="K68" s="95"/>
+      <c r="L68" s="95"/>
+      <c r="M68" s="95"/>
+      <c r="N68" s="96"/>
+      <c r="O68" s="95"/>
+      <c r="P68" s="95"/>
+      <c r="Q68" s="95"/>
+      <c r="R68" s="134"/>
+      <c r="S68" s="95"/>
+      <c r="T68" s="95"/>
+      <c r="U68" s="95"/>
+      <c r="V68" s="96"/>
+      <c r="W68" s="95"/>
+      <c r="X68" s="158"/>
+      <c r="Y68" s="95"/>
+      <c r="Z68" s="96"/>
+      <c r="AA68" s="97"/>
+      <c r="AB68" s="98"/>
+    </row>
+    <row r="69" spans="1:28" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="156" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69" s="156"/>
+      <c r="C69" s="99">
+        <f>SUM(C10:C68)</f>
+        <v>109.5</v>
+      </c>
+      <c r="D69" s="99">
+        <f>SUM(D10:D68)</f>
+        <v>88</v>
+      </c>
+      <c r="E69" s="99">
+        <f>SUM(E10:E68)</f>
+        <v>92.25</v>
+      </c>
+      <c r="F69" s="99">
+        <f>SUM(F10:F68)</f>
+        <v>108</v>
+      </c>
+      <c r="G69" s="100"/>
+      <c r="H69" s="99"/>
+      <c r="I69" s="101"/>
+      <c r="J69" s="99">
+        <f>SUM(C69:F69)</f>
+        <v>397.75</v>
+      </c>
+      <c r="K69" s="102"/>
+      <c r="L69" s="102"/>
+      <c r="M69" s="102"/>
+      <c r="N69" s="102"/>
+      <c r="O69" s="102"/>
+      <c r="P69" s="102"/>
+      <c r="Q69" s="102"/>
+      <c r="R69" s="102"/>
+      <c r="S69" s="102"/>
+      <c r="T69" s="102"/>
+      <c r="U69" s="102"/>
+      <c r="V69" s="102"/>
+      <c r="W69" s="102"/>
+      <c r="X69" s="102"/>
+      <c r="Y69" s="102"/>
+      <c r="Z69" s="102"/>
+      <c r="AA69" s="132">
+        <f>SUM(AA10:AA68)</f>
+        <v>0.25</v>
+      </c>
+      <c r="AB69" s="133"/>
+    </row>
+    <row r="70" spans="1:28" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="151" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B70" s="151"/>
       <c r="C70" s="99">
-        <f>SUM(C10:C69)</f>
-        <v>109.5</v>
+        <f>135-C69</f>
+        <v>25.5</v>
       </c>
       <c r="D70" s="99">
-        <f>SUM(D10:D69)</f>
-        <v>88</v>
+        <f>135-D69</f>
+        <v>47</v>
       </c>
       <c r="E70" s="99">
-        <f>SUM(E10:E69)</f>
-        <v>90.75</v>
+        <f>135-E69</f>
+        <v>42.75</v>
       </c>
       <c r="F70" s="99">
-        <f>SUM(F10:F69)</f>
-        <v>108</v>
+        <f>135-F69</f>
+        <v>27</v>
       </c>
       <c r="G70" s="100"/>
       <c r="H70" s="99"/>
-      <c r="I70" s="101"/>
+      <c r="I70" s="99"/>
       <c r="J70" s="99">
         <f>SUM(C70:F70)</f>
-        <v>396.25</v>
+        <v>142.25</v>
       </c>
       <c r="K70" s="102"/>
       <c r="L70" s="102"/>
@@ -5857,39 +5912,24 @@
       <c r="X70" s="102"/>
       <c r="Y70" s="102"/>
       <c r="Z70" s="102"/>
-      <c r="AA70" s="137">
-        <f>SUM(AA10:AA69)</f>
-        <v>0.25</v>
-      </c>
-      <c r="AB70" s="138"/>
-    </row>
-    <row r="71" spans="1:28" ht="16.95" customHeight="1" thickBot="1">
-      <c r="A71" s="146" t="s">
-        <v>69</v>
-      </c>
-      <c r="B71" s="146"/>
-      <c r="C71" s="99">
-        <f>135-C70</f>
-        <v>25.5</v>
-      </c>
-      <c r="D71" s="99">
-        <f>135-D70</f>
-        <v>47</v>
-      </c>
-      <c r="E71" s="99">
-        <f>135-E70</f>
-        <v>44.25</v>
-      </c>
-      <c r="F71" s="99">
-        <f>135-F70</f>
-        <v>27</v>
-      </c>
-      <c r="G71" s="100"/>
+      <c r="AA70" s="102"/>
+      <c r="AB70" s="102"/>
+    </row>
+    <row r="71" spans="1:28" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="152" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71" s="152"/>
+      <c r="C71" s="99"/>
+      <c r="D71" s="99"/>
+      <c r="E71" s="99"/>
+      <c r="F71" s="99"/>
+      <c r="G71" s="99"/>
       <c r="H71" s="99"/>
       <c r="I71" s="99"/>
       <c r="J71" s="99">
-        <f>SUM(C71:F71)</f>
-        <v>143.75</v>
+        <f>C71+D71+F71+E71</f>
+        <v>0</v>
       </c>
       <c r="K71" s="102"/>
       <c r="L71" s="102"/>
@@ -5910,21 +5950,24 @@
       <c r="AA71" s="102"/>
       <c r="AB71" s="102"/>
     </row>
-    <row r="72" spans="1:28" ht="16.95" customHeight="1">
-      <c r="A72" s="147" t="s">
-        <v>70</v>
-      </c>
-      <c r="B72" s="147"/>
+    <row r="72" spans="1:28" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="151" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" s="151"/>
       <c r="C72" s="99"/>
       <c r="D72" s="99"/>
-      <c r="E72" s="99"/>
+      <c r="E72" s="103"/>
       <c r="F72" s="99"/>
       <c r="G72" s="99"/>
       <c r="H72" s="99"/>
-      <c r="I72" s="99"/>
+      <c r="I72" s="104">
+        <f>SUM(I10:I68)</f>
+        <v>399.25</v>
+      </c>
       <c r="J72" s="99">
-        <f>C72+D72+F72+E72</f>
-        <v>0</v>
+        <f>SUM(J10:J68)</f>
+        <v>397.75</v>
       </c>
       <c r="K72" s="102"/>
       <c r="L72" s="102"/>
@@ -5945,25 +5988,17 @@
       <c r="AA72" s="102"/>
       <c r="AB72" s="102"/>
     </row>
-    <row r="73" spans="1:28" ht="16.95" customHeight="1">
-      <c r="A73" s="146" t="s">
-        <v>71</v>
-      </c>
-      <c r="B73" s="146"/>
-      <c r="C73" s="99"/>
-      <c r="D73" s="99"/>
-      <c r="E73" s="103"/>
-      <c r="F73" s="99"/>
-      <c r="G73" s="99"/>
-      <c r="H73" s="99"/>
-      <c r="I73" s="104">
-        <f>SUM(I10:I69)</f>
-        <v>404.25</v>
-      </c>
-      <c r="J73" s="99">
-        <f>SUM(J10:J69)</f>
-        <v>396.25</v>
-      </c>
+    <row r="73" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="105"/>
+      <c r="B73" s="105"/>
+      <c r="C73" s="106"/>
+      <c r="D73" s="106"/>
+      <c r="E73" s="106"/>
+      <c r="F73" s="106"/>
+      <c r="G73" s="106"/>
+      <c r="H73" s="106"/>
+      <c r="I73" s="106"/>
+      <c r="J73" s="106"/>
       <c r="K73" s="102"/>
       <c r="L73" s="102"/>
       <c r="M73" s="102"/>
@@ -5983,10 +6018,15 @@
       <c r="AA73" s="102"/>
       <c r="AB73" s="102"/>
     </row>
-    <row r="74" spans="1:28" ht="15.6">
-      <c r="A74" s="105"/>
-      <c r="B74" s="105"/>
-      <c r="C74" s="106"/>
+    <row r="74" spans="1:28" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="152" t="s">
+        <v>72</v>
+      </c>
+      <c r="B74" s="152"/>
+      <c r="C74" s="99">
+        <f>135*4</f>
+        <v>540</v>
+      </c>
       <c r="D74" s="106"/>
       <c r="E74" s="106"/>
       <c r="F74" s="106"/>
@@ -6013,14 +6053,14 @@
       <c r="AA74" s="102"/>
       <c r="AB74" s="102"/>
     </row>
-    <row r="75" spans="1:28" ht="16.2" customHeight="1">
-      <c r="A75" s="147" t="s">
-        <v>72</v>
-      </c>
-      <c r="B75" s="147"/>
+    <row r="75" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="153" t="s">
+        <v>73</v>
+      </c>
+      <c r="B75" s="153"/>
       <c r="C75" s="99">
-        <f>135*4</f>
-        <v>540</v>
+        <f>C74-J72</f>
+        <v>142.25</v>
       </c>
       <c r="D75" s="106"/>
       <c r="E75" s="106"/>
@@ -6048,61 +6088,40 @@
       <c r="AA75" s="102"/>
       <c r="AB75" s="102"/>
     </row>
-    <row r="76" spans="1:28" ht="15.6">
-      <c r="A76" s="148" t="s">
-        <v>73</v>
-      </c>
-      <c r="B76" s="148"/>
-      <c r="C76" s="99">
-        <f>C75-J73</f>
-        <v>143.75</v>
-      </c>
-      <c r="D76" s="106"/>
-      <c r="E76" s="106"/>
-      <c r="F76" s="106"/>
-      <c r="G76" s="106"/>
-      <c r="H76" s="106"/>
-      <c r="I76" s="106"/>
-      <c r="J76" s="106"/>
-      <c r="K76" s="102"/>
-      <c r="L76" s="102"/>
-      <c r="M76" s="102"/>
-      <c r="N76" s="102"/>
-      <c r="O76" s="102"/>
-      <c r="P76" s="102"/>
-      <c r="Q76" s="102"/>
-      <c r="R76" s="102"/>
-      <c r="S76" s="102"/>
-      <c r="T76" s="102"/>
-      <c r="U76" s="102"/>
-      <c r="V76" s="102"/>
-      <c r="W76" s="102"/>
-      <c r="X76" s="102"/>
-      <c r="Y76" s="102"/>
-      <c r="Z76" s="102"/>
+    <row r="76" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="107"/>
+      <c r="B76" s="105"/>
+      <c r="C76" s="108"/>
+      <c r="D76" s="108"/>
+      <c r="E76" s="108"/>
+      <c r="F76" s="108"/>
+      <c r="G76" s="105"/>
+      <c r="H76" s="109"/>
+      <c r="I76" s="110"/>
+      <c r="J76" s="110"/>
       <c r="AA76" s="102"/>
-      <c r="AB76" s="102"/>
-    </row>
-    <row r="77" spans="1:28" ht="15.6">
-      <c r="A77" s="107"/>
-      <c r="B77" s="105"/>
-      <c r="C77" s="108"/>
-      <c r="D77" s="108"/>
-      <c r="E77" s="108"/>
-      <c r="F77" s="108"/>
-      <c r="G77" s="105"/>
-      <c r="H77" s="109"/>
-      <c r="I77" s="110"/>
-      <c r="J77" s="110"/>
-      <c r="AA77" s="102"/>
-    </row>
-    <row r="78" spans="1:28">
-      <c r="D78" s="111"/>
-      <c r="E78" s="111"/>
-      <c r="F78" s="111"/>
-    </row>
-    <row r="79" spans="1:28" s="113" customFormat="1" ht="13.8">
-      <c r="A79" s="112"/>
+    </row>
+    <row r="77" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="D77" s="111"/>
+      <c r="E77" s="111"/>
+      <c r="F77" s="111"/>
+    </row>
+    <row r="78" spans="1:28" s="113" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A78" s="112"/>
+      <c r="C78" s="114"/>
+      <c r="D78" s="114"/>
+      <c r="E78" s="114"/>
+      <c r="F78" s="114"/>
+      <c r="H78" s="115"/>
+      <c r="I78" s="116"/>
+      <c r="J78" s="116"/>
+      <c r="N78" s="117"/>
+      <c r="R78" s="117"/>
+      <c r="V78" s="117"/>
+      <c r="Z78" s="117"/>
+      <c r="AA78" s="118"/>
+    </row>
+    <row r="79" spans="1:28" s="113" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="C79" s="114"/>
       <c r="D79" s="114"/>
       <c r="E79" s="114"/>
@@ -6116,7 +6135,7 @@
       <c r="Z79" s="117"/>
       <c r="AA79" s="118"/>
     </row>
-    <row r="80" spans="1:28" s="113" customFormat="1" ht="13.8">
+    <row r="80" spans="1:28" s="113" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="C80" s="114"/>
       <c r="D80" s="114"/>
       <c r="E80" s="114"/>
@@ -6130,27 +6149,16 @@
       <c r="Z80" s="117"/>
       <c r="AA80" s="118"/>
     </row>
-    <row r="81" spans="3:27" s="113" customFormat="1" ht="13.8">
-      <c r="C81" s="114"/>
-      <c r="D81" s="114"/>
-      <c r="E81" s="114"/>
-      <c r="F81" s="114"/>
-      <c r="H81" s="115"/>
-      <c r="I81" s="116"/>
-      <c r="J81" s="116"/>
-      <c r="N81" s="117"/>
-      <c r="R81" s="117"/>
-      <c r="V81" s="117"/>
-      <c r="Z81" s="117"/>
-      <c r="AA81" s="118"/>
-    </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
     <mergeCell ref="S6:V6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
@@ -6160,129 +6168,137 @@
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="K7:Z7"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K6:R6"/>
   </mergeCells>
   <conditionalFormatting sqref="H19">
-    <cfRule type="containsText" dxfId="41" priority="19" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="44" priority="26" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",H19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H45 H49 H47">
-    <cfRule type="containsText" dxfId="40" priority="20" operator="containsText" text="En attente">
+    <cfRule type="containsText" dxfId="43" priority="27" operator="containsText" text="En attente">
       <formula>NOT(ISERROR(SEARCH("En attente",H9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="21" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="42" priority="28" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",H9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="22" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="41" priority="29" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",H9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9:F45 C49:F49 C47:F47 C57:F69">
-    <cfRule type="cellIs" dxfId="37" priority="23" operator="equal">
+  <conditionalFormatting sqref="C9:F45 C47:F47 C56:F64 C49:F54 C66:F68">
+    <cfRule type="cellIs" dxfId="40" priority="30" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="24">
+    <cfRule type="expression" dxfId="39" priority="31">
       <formula>$H9="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9:F45 C49:F49 C47:F47 C57:F69">
-    <cfRule type="expression" dxfId="35" priority="25">
+  <conditionalFormatting sqref="C9:F45 C47:F47 C56:F64 C49:F54 C66:F68">
+    <cfRule type="expression" dxfId="38" priority="32">
       <formula>$H9="En cours"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="26">
+    <cfRule type="expression" dxfId="37" priority="33">
       <formula>$H9="En attente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="containsText" dxfId="33" priority="27" operator="containsText" text="En attente">
+    <cfRule type="containsText" dxfId="36" priority="34" operator="containsText" text="En attente">
       <formula>NOT(ISERROR(SEARCH("En attente",H48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="28" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="35" priority="35" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",H48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="29" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="34" priority="36" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",H48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:F48">
-    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="37" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="31">
+    <cfRule type="expression" dxfId="32" priority="38">
       <formula>$H48="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:F48">
-    <cfRule type="expression" dxfId="28" priority="32">
+    <cfRule type="expression" dxfId="31" priority="39">
       <formula>$H48="En cours"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="33">
+    <cfRule type="expression" dxfId="30" priority="40">
       <formula>$H48="En attente"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H50:H55">
-    <cfRule type="containsText" dxfId="26" priority="34" operator="containsText" text="En attente">
+  <conditionalFormatting sqref="H50:H54">
+    <cfRule type="containsText" dxfId="29" priority="41" operator="containsText" text="En attente">
       <formula>NOT(ISERROR(SEARCH("En attente",H50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="35" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="28" priority="42" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",H50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="36" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="27" priority="43" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",H50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50:F55">
-    <cfRule type="cellIs" dxfId="23" priority="37" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="38">
-      <formula>$H50="Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50:F55">
-    <cfRule type="expression" dxfId="21" priority="39">
-      <formula>$H50="En cours"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="40">
-      <formula>$H50="En attente"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H46">
-    <cfRule type="containsText" dxfId="19" priority="41" operator="containsText" text="En attente">
+    <cfRule type="containsText" dxfId="26" priority="48" operator="containsText" text="En attente">
       <formula>NOT(ISERROR(SEARCH("En attente",H46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="42" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="25" priority="49" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",H46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="43" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="24" priority="50" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",H46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:F46">
-    <cfRule type="cellIs" dxfId="16" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="51" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="45">
+    <cfRule type="expression" dxfId="22" priority="52">
       <formula>$H46="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:F46">
-    <cfRule type="expression" dxfId="14" priority="46">
+    <cfRule type="expression" dxfId="21" priority="53">
       <formula>$H46="En cours"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="47">
+    <cfRule type="expression" dxfId="20" priority="54">
       <formula>$H46="En attente"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H56">
+  <conditionalFormatting sqref="H55">
+    <cfRule type="containsText" dxfId="19" priority="18" operator="containsText" text="En attente">
+      <formula>NOT(ISERROR(SEARCH("En attente",H55)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",H55)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="20" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",H55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:F55">
+    <cfRule type="cellIs" dxfId="16" priority="21" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="22">
+      <formula>$H55="Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:F55">
+    <cfRule type="expression" dxfId="14" priority="23">
+      <formula>$H55="En cours"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="24">
+      <formula>$H55="En attente"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H56:H61">
     <cfRule type="containsText" dxfId="12" priority="11" operator="containsText" text="En attente">
       <formula>NOT(ISERROR(SEARCH("En attente",H56)))</formula>
     </cfRule>
@@ -6293,46 +6309,46 @@
       <formula>NOT(ISERROR(SEARCH("Terminé",H56)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56:F56">
-    <cfRule type="cellIs" dxfId="9" priority="14" operator="equal">
+  <conditionalFormatting sqref="H62:H64 H66:H68">
+    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="En attente">
+      <formula>NOT(ISERROR(SEARCH("En attente",H62)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",H62)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",H62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65:F65">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="15">
-      <formula>$H56="Terminé"</formula>
+    <cfRule type="expression" dxfId="5" priority="5">
+      <formula>$H65="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56:F56">
-    <cfRule type="expression" dxfId="7" priority="16">
-      <formula>$H56="En cours"</formula>
+  <conditionalFormatting sqref="C65:F65">
+    <cfRule type="expression" dxfId="4" priority="6">
+      <formula>$H65="En cours"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="17">
-      <formula>$H56="En attente"</formula>
+    <cfRule type="expression" dxfId="3" priority="7">
+      <formula>$H65="En attente"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H57:H62">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="En attente">
-      <formula>NOT(ISERROR(SEARCH("En attente",H57)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",H57)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",H57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H63:H69">
+  <conditionalFormatting sqref="H65">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="En attente">
-      <formula>NOT(ISERROR(SEARCH("En attente",H63)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En attente",H65)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",H63)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",H65)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",H63)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",H65)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H9:H69">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H9:H68" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"En attente,En cours,Terminé"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6344,19 +6360,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK3"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1025" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="119" t="s">
         <v>6</v>
       </c>
@@ -6364,7 +6380,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -6372,7 +6388,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -6387,12 +6403,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMK1"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1025" width="10.6640625" style="1"/>
   </cols>

</xml_diff>

<commit_message>
ajout des heures redaction sprint
</commit_message>
<xml_diff>
--- a/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire copy.xlsx
+++ b/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire copy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alxbo\Source\Repos\mrjrdg\marque-sans-nom\Semainiers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Desktop/marque-sans-nom/Semainiers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B40382-F080-4DEA-B9D8-2FC2EE8A7683}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D2F4B0-F5D1-4144-B8B2-CFEF80DE356A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="18740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -1514,35 +1512,21 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="19" fillId="0" borderId="20" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="19" fillId="0" borderId="8" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="15" xfId="10" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="22" xfId="10" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1560,35 +1544,49 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="19" fillId="0" borderId="20" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="19" fillId="0" borderId="8" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="15" xfId="10" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="22" xfId="10" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
+    <cellStyle name="Bad" xfId="10" builtinId="27"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Excel Built-in 60% - Accent4" xfId="7" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Excel Built-in Bad" xfId="6" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Excel Built-in Good" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Excel Built-in Neutral" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Excel Built-in Normal" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Insatisfaisant" xfId="10" builtinId="27"/>
-    <cellStyle name="Milliers" xfId="1" builtinId="3"/>
-    <cellStyle name="Neutre" xfId="9" builtinId="28"/>
+    <cellStyle name="Good" xfId="8" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="9" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Satisfaisant" xfId="8" builtinId="26"/>
   </cellStyles>
   <dxfs count="45">
     <dxf>
@@ -2112,7 +2110,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2154,7 +2152,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2206,7 +2204,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2413,19 +2411,19 @@
   </sheetPr>
   <dimension ref="A1:AMK80"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="74.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="74.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" style="2" customWidth="1"/>
-    <col min="4" max="5" width="8.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.1640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="3" customWidth="1"/>
     <col min="9" max="10" width="9.33203125" style="4" customWidth="1"/>
     <col min="11" max="13" width="8" style="1" customWidth="1"/>
     <col min="14" max="14" width="8" style="5" customWidth="1"/>
@@ -2441,23 +2439,23 @@
     <col min="29" max="1025" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="8" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="141" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="141"/>
+    <row r="1" spans="1:28" s="8" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="159" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="159"/>
       <c r="C1" s="7"/>
-      <c r="D1" s="142" t="s">
+      <c r="D1" s="160" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="142"/>
-      <c r="F1" s="142"/>
-      <c r="G1" s="142"/>
-      <c r="H1" s="142"/>
-      <c r="I1" s="142"/>
-      <c r="J1" s="142"/>
-      <c r="K1" s="142"/>
-      <c r="L1" s="142"/>
+      <c r="E1" s="160"/>
+      <c r="F1" s="160"/>
+      <c r="G1" s="160"/>
+      <c r="H1" s="160"/>
+      <c r="I1" s="160"/>
+      <c r="J1" s="160"/>
+      <c r="K1" s="160"/>
+      <c r="L1" s="160"/>
       <c r="N1" s="3"/>
       <c r="P1" s="9"/>
       <c r="Q1" s="8" t="s">
@@ -2468,21 +2466,21 @@
       <c r="Z1" s="3"/>
       <c r="AA1" s="10"/>
     </row>
-    <row r="2" spans="1:28" s="8" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="141" t="s">
+    <row r="2" spans="1:28" s="8" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="141"/>
+      <c r="B2" s="159"/>
       <c r="C2" s="7"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
-      <c r="F2" s="141" t="s">
+      <c r="F2" s="159" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="141"/>
-      <c r="H2" s="141"/>
-      <c r="I2" s="141"/>
-      <c r="J2" s="141"/>
+      <c r="G2" s="159"/>
+      <c r="H2" s="159"/>
+      <c r="I2" s="159"/>
+      <c r="J2" s="159"/>
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
       <c r="N2" s="3"/>
@@ -2495,7 +2493,7 @@
       <c r="Z2" s="3"/>
       <c r="AA2" s="10"/>
     </row>
-    <row r="3" spans="1:28" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -2513,7 +2511,7 @@
       <c r="Z3" s="3"/>
       <c r="AA3" s="10"/>
     </row>
-    <row r="4" spans="1:28" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
@@ -2533,7 +2531,7 @@
       <c r="Z4" s="3"/>
       <c r="AA4" s="10"/>
     </row>
-    <row r="5" spans="1:28" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
@@ -2557,7 +2555,7 @@
       </c>
       <c r="AA5" s="10"/>
     </row>
-    <row r="6" spans="1:28" s="8" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" s="8" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
@@ -2565,78 +2563,78 @@
       <c r="H6" s="3"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="143" t="s">
+      <c r="K6" s="151" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="143"/>
-      <c r="M6" s="143"/>
-      <c r="N6" s="143"/>
-      <c r="O6" s="143"/>
-      <c r="P6" s="143"/>
-      <c r="Q6" s="143"/>
-      <c r="R6" s="143"/>
-      <c r="S6" s="143" t="s">
+      <c r="L6" s="151"/>
+      <c r="M6" s="151"/>
+      <c r="N6" s="151"/>
+      <c r="O6" s="151"/>
+      <c r="P6" s="151"/>
+      <c r="Q6" s="151"/>
+      <c r="R6" s="151"/>
+      <c r="S6" s="151" t="s">
         <v>10</v>
       </c>
-      <c r="T6" s="143"/>
-      <c r="U6" s="143"/>
-      <c r="V6" s="143"/>
+      <c r="T6" s="151"/>
+      <c r="U6" s="151"/>
+      <c r="V6" s="151"/>
       <c r="Z6" s="17"/>
       <c r="AA6" s="10"/>
     </row>
-    <row r="7" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="144" t="s">
+    <row r="7" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="152" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="145" t="s">
+      <c r="B7" s="153" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="146" t="s">
+      <c r="C7" s="154" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="146"/>
-      <c r="E7" s="146"/>
-      <c r="F7" s="146"/>
-      <c r="G7" s="147" t="s">
+      <c r="D7" s="154"/>
+      <c r="E7" s="154"/>
+      <c r="F7" s="154"/>
+      <c r="G7" s="155" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="148" t="s">
+      <c r="H7" s="156" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="149" t="s">
+      <c r="I7" s="157" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="149" t="s">
+      <c r="J7" s="157" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="150" t="s">
+      <c r="K7" s="158" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="150"/>
-      <c r="M7" s="150"/>
-      <c r="N7" s="150"/>
-      <c r="O7" s="150"/>
-      <c r="P7" s="150"/>
-      <c r="Q7" s="150"/>
-      <c r="R7" s="150"/>
-      <c r="S7" s="150"/>
-      <c r="T7" s="150"/>
-      <c r="U7" s="150"/>
-      <c r="V7" s="150"/>
-      <c r="W7" s="150"/>
-      <c r="X7" s="150"/>
-      <c r="Y7" s="150"/>
-      <c r="Z7" s="150"/>
-      <c r="AA7" s="154" t="s">
+      <c r="L7" s="158"/>
+      <c r="M7" s="158"/>
+      <c r="N7" s="158"/>
+      <c r="O7" s="158"/>
+      <c r="P7" s="158"/>
+      <c r="Q7" s="158"/>
+      <c r="R7" s="158"/>
+      <c r="S7" s="158"/>
+      <c r="T7" s="158"/>
+      <c r="U7" s="158"/>
+      <c r="V7" s="158"/>
+      <c r="W7" s="158"/>
+      <c r="X7" s="158"/>
+      <c r="Y7" s="158"/>
+      <c r="Z7" s="158"/>
+      <c r="AA7" s="148" t="s">
         <v>19</v>
       </c>
-      <c r="AB7" s="155" t="s">
+      <c r="AB7" s="149" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="144"/>
-      <c r="B8" s="145"/>
+    <row r="8" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="152"/>
+      <c r="B8" s="153"/>
       <c r="C8" s="20" t="s">
         <v>21</v>
       </c>
@@ -2649,10 +2647,10 @@
       <c r="F8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="147"/>
-      <c r="H8" s="148"/>
-      <c r="I8" s="149"/>
-      <c r="J8" s="149"/>
+      <c r="G8" s="155"/>
+      <c r="H8" s="156"/>
+      <c r="I8" s="157"/>
+      <c r="J8" s="157"/>
       <c r="K8" s="21">
         <v>43838</v>
       </c>
@@ -2716,10 +2714,10 @@
         <f t="shared" si="0"/>
         <v>43943</v>
       </c>
-      <c r="AA8" s="154"/>
-      <c r="AB8" s="155"/>
-    </row>
-    <row r="9" spans="1:28" ht="18" x14ac:dyDescent="0.3">
+      <c r="AA8" s="148"/>
+      <c r="AB8" s="149"/>
+    </row>
+    <row r="9" spans="1:28" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>25</v>
@@ -2751,7 +2749,7 @@
       <c r="AA9" s="33"/>
       <c r="AB9" s="34"/>
     </row>
-    <row r="10" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="35">
         <v>1</v>
       </c>
@@ -2806,7 +2804,7 @@
       </c>
       <c r="AB10" s="45"/>
     </row>
-    <row r="11" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="35">
         <v>2</v>
       </c>
@@ -2861,7 +2859,7 @@
       </c>
       <c r="AB11" s="48"/>
     </row>
-    <row r="12" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="35">
         <v>3</v>
       </c>
@@ -2915,7 +2913,7 @@
       </c>
       <c r="AB12" s="49"/>
     </row>
-    <row r="13" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="35">
         <v>4</v>
       </c>
@@ -2970,7 +2968,7 @@
       </c>
       <c r="AB13" s="48"/>
     </row>
-    <row r="14" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="35">
         <v>5</v>
       </c>
@@ -3025,7 +3023,7 @@
       </c>
       <c r="AB14" s="48"/>
     </row>
-    <row r="15" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="35">
         <v>6</v>
       </c>
@@ -3080,7 +3078,7 @@
       </c>
       <c r="AB15" s="48"/>
     </row>
-    <row r="16" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="35">
         <v>7</v>
       </c>
@@ -3135,7 +3133,7 @@
       </c>
       <c r="AB16" s="48"/>
     </row>
-    <row r="17" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="35">
         <v>8</v>
       </c>
@@ -3190,7 +3188,7 @@
       </c>
       <c r="AB17" s="48"/>
     </row>
-    <row r="18" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="35">
         <v>9</v>
       </c>
@@ -3245,7 +3243,7 @@
       </c>
       <c r="AB18" s="48"/>
     </row>
-    <row r="19" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="35">
         <v>10</v>
       </c>
@@ -3300,7 +3298,7 @@
       </c>
       <c r="AB19" s="48"/>
     </row>
-    <row r="20" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="35">
         <v>11</v>
       </c>
@@ -3355,7 +3353,7 @@
       </c>
       <c r="AB20" s="48"/>
     </row>
-    <row r="21" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="35">
         <v>12</v>
       </c>
@@ -3410,7 +3408,7 @@
       </c>
       <c r="AB21" s="48"/>
     </row>
-    <row r="22" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="35">
         <v>13</v>
       </c>
@@ -3465,7 +3463,7 @@
       </c>
       <c r="AB22" s="48"/>
     </row>
-    <row r="23" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="35">
         <v>14</v>
       </c>
@@ -3520,7 +3518,7 @@
       </c>
       <c r="AB23" s="48"/>
     </row>
-    <row r="24" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="35">
         <v>15</v>
       </c>
@@ -3575,7 +3573,7 @@
       </c>
       <c r="AB24" s="48"/>
     </row>
-    <row r="25" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="35">
         <v>16</v>
       </c>
@@ -3630,7 +3628,7 @@
       </c>
       <c r="AB25" s="48"/>
     </row>
-    <row r="26" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="35">
         <v>17</v>
       </c>
@@ -3685,7 +3683,7 @@
       </c>
       <c r="AB26" s="76"/>
     </row>
-    <row r="27" spans="1:28" s="79" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" s="79" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="35">
         <v>18</v>
       </c>
@@ -3740,7 +3738,7 @@
       </c>
       <c r="AB27" s="48"/>
     </row>
-    <row r="28" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="35">
         <v>19</v>
       </c>
@@ -3795,7 +3793,7 @@
       </c>
       <c r="AB28" s="48"/>
     </row>
-    <row r="29" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="35">
         <v>20</v>
       </c>
@@ -3850,7 +3848,7 @@
       </c>
       <c r="AB29" s="48"/>
     </row>
-    <row r="30" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="35">
         <v>21</v>
       </c>
@@ -3905,7 +3903,7 @@
       </c>
       <c r="AB30" s="48"/>
     </row>
-    <row r="31" spans="1:28" s="79" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:28" s="79" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="35">
         <v>22</v>
       </c>
@@ -3960,7 +3958,7 @@
       </c>
       <c r="AB31" s="48"/>
     </row>
-    <row r="32" spans="1:28" s="79" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:28" s="79" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="35">
         <v>23</v>
       </c>
@@ -4015,7 +4013,7 @@
       </c>
       <c r="AB32" s="48"/>
     </row>
-    <row r="33" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="35">
         <v>24</v>
       </c>
@@ -4070,7 +4068,7 @@
       </c>
       <c r="AB33" s="48"/>
     </row>
-    <row r="34" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="35">
         <v>25</v>
       </c>
@@ -4125,7 +4123,7 @@
       </c>
       <c r="AB34" s="48"/>
     </row>
-    <row r="35" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="35">
         <v>27</v>
       </c>
@@ -4178,7 +4176,7 @@
       </c>
       <c r="AB35" s="48"/>
     </row>
-    <row r="36" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="35">
         <v>28</v>
       </c>
@@ -4231,7 +4229,7 @@
       </c>
       <c r="AB36" s="48"/>
     </row>
-    <row r="37" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="35">
         <v>29</v>
       </c>
@@ -4284,7 +4282,7 @@
       </c>
       <c r="AB37" s="48"/>
     </row>
-    <row r="38" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="35">
         <v>30</v>
       </c>
@@ -4337,7 +4335,7 @@
       </c>
       <c r="AB38" s="48"/>
     </row>
-    <row r="39" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="35">
         <v>31</v>
       </c>
@@ -4390,7 +4388,7 @@
       </c>
       <c r="AB39" s="48"/>
     </row>
-    <row r="40" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="35">
         <v>32</v>
       </c>
@@ -4443,7 +4441,7 @@
       </c>
       <c r="AB40" s="48"/>
     </row>
-    <row r="41" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="35">
         <v>33</v>
       </c>
@@ -4498,7 +4496,7 @@
       </c>
       <c r="AB41" s="48"/>
     </row>
-    <row r="42" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="35">
         <v>34</v>
       </c>
@@ -4551,7 +4549,7 @@
       </c>
       <c r="AB42" s="48"/>
     </row>
-    <row r="43" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="35">
         <v>35</v>
       </c>
@@ -4606,7 +4604,7 @@
       </c>
       <c r="AB43" s="48"/>
     </row>
-    <row r="44" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="35">
         <v>36</v>
       </c>
@@ -4661,7 +4659,7 @@
       </c>
       <c r="AB44" s="48"/>
     </row>
-    <row r="45" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="35">
         <v>37</v>
       </c>
@@ -4714,7 +4712,7 @@
       </c>
       <c r="AB45" s="48"/>
     </row>
-    <row r="46" spans="1:28" s="86" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:28" s="86" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="35">
         <v>39</v>
       </c>
@@ -4766,7 +4764,7 @@
       <c r="AA46" s="44"/>
       <c r="AB46" s="48"/>
     </row>
-    <row r="47" spans="1:28" s="86" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:28" s="86" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="35">
         <v>40</v>
       </c>
@@ -4818,7 +4816,7 @@
       <c r="AA47" s="44"/>
       <c r="AB47" s="48"/>
     </row>
-    <row r="48" spans="1:28" s="46" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:28" s="46" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A48" s="87"/>
       <c r="B48" s="24" t="s">
         <v>64</v>
@@ -4850,7 +4848,7 @@
       <c r="AA48" s="90"/>
       <c r="AB48" s="91"/>
     </row>
-    <row r="49" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="35">
         <v>1</v>
       </c>
@@ -4905,7 +4903,7 @@
       </c>
       <c r="AB49" s="48"/>
     </row>
-    <row r="50" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="35">
         <v>2</v>
       </c>
@@ -4958,7 +4956,7 @@
       </c>
       <c r="AB50" s="48"/>
     </row>
-    <row r="51" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="35">
         <v>3</v>
       </c>
@@ -5008,7 +5006,7 @@
       <c r="AA51" s="94"/>
       <c r="AB51" s="76"/>
     </row>
-    <row r="52" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="35">
         <v>4</v>
       </c>
@@ -5060,11 +5058,11 @@
       <c r="AA52" s="94"/>
       <c r="AB52" s="76"/>
     </row>
-    <row r="53" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="159">
+    <row r="53" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" s="143">
         <v>5</v>
       </c>
-      <c r="B53" s="160" t="s">
+      <c r="B53" s="144" t="s">
         <v>79</v>
       </c>
       <c r="C53" s="37">
@@ -5112,7 +5110,7 @@
       <c r="AA53" s="94"/>
       <c r="AB53" s="76"/>
     </row>
-    <row r="54" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="35">
         <v>6</v>
       </c>
@@ -5164,7 +5162,7 @@
       <c r="AA54" s="94"/>
       <c r="AB54" s="76"/>
     </row>
-    <row r="55" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="35">
         <v>7</v>
       </c>
@@ -5216,7 +5214,7 @@
       <c r="AA55" s="94"/>
       <c r="AB55" s="76"/>
     </row>
-    <row r="56" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="35">
         <v>8</v>
       </c>
@@ -5268,7 +5266,7 @@
       <c r="AA56" s="94"/>
       <c r="AB56" s="76"/>
     </row>
-    <row r="57" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="35">
         <v>9</v>
       </c>
@@ -5320,7 +5318,7 @@
       <c r="AA57" s="94"/>
       <c r="AB57" s="76"/>
     </row>
-    <row r="58" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="35">
         <v>10</v>
       </c>
@@ -5372,7 +5370,7 @@
       <c r="AA58" s="94"/>
       <c r="AB58" s="76"/>
     </row>
-    <row r="59" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="35">
         <v>11</v>
       </c>
@@ -5424,7 +5422,7 @@
       <c r="AA59" s="94"/>
       <c r="AB59" s="76"/>
     </row>
-    <row r="60" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="35">
         <v>12</v>
       </c>
@@ -5476,7 +5474,7 @@
       <c r="AA60" s="94"/>
       <c r="AB60" s="76"/>
     </row>
-    <row r="61" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="35">
         <v>13</v>
       </c>
@@ -5528,7 +5526,7 @@
       <c r="AA61" s="94"/>
       <c r="AB61" s="76"/>
     </row>
-    <row r="62" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="35">
         <v>14</v>
       </c>
@@ -5580,7 +5578,7 @@
       <c r="AA62" s="94"/>
       <c r="AB62" s="76"/>
     </row>
-    <row r="63" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="35">
         <v>15</v>
       </c>
@@ -5632,11 +5630,11 @@
       <c r="AA63" s="94"/>
       <c r="AB63" s="76"/>
     </row>
-    <row r="64" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="159">
+    <row r="64" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" s="143">
         <v>17</v>
       </c>
-      <c r="B64" s="160" t="s">
+      <c r="B64" s="144" t="s">
         <v>86</v>
       </c>
       <c r="C64" s="37">
@@ -5679,7 +5677,7 @@
       <c r="AA64" s="94"/>
       <c r="AB64" s="76"/>
     </row>
-    <row r="65" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="35">
         <v>18</v>
       </c>
@@ -5687,7 +5685,7 @@
         <v>85</v>
       </c>
       <c r="C65" s="37">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="D65" s="37">
         <v>0</v>
@@ -5707,7 +5705,7 @@
       </c>
       <c r="J65" s="40">
         <f t="shared" ref="J65" si="5">SUM(C65:F65)</f>
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="K65" s="73"/>
       <c r="L65" s="73"/>
@@ -5728,7 +5726,7 @@
       <c r="AA65" s="94"/>
       <c r="AB65" s="76"/>
     </row>
-    <row r="66" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="35"/>
       <c r="B66" s="69"/>
       <c r="C66" s="37"/>
@@ -5752,13 +5750,13 @@
       <c r="U66" s="73"/>
       <c r="V66" s="52"/>
       <c r="W66" s="73"/>
-      <c r="X66" s="157"/>
+      <c r="X66" s="141"/>
       <c r="Y66" s="73"/>
       <c r="Z66" s="52"/>
       <c r="AA66" s="94"/>
       <c r="AB66" s="76"/>
     </row>
-    <row r="67" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="35"/>
       <c r="B67" s="69"/>
       <c r="C67" s="37"/>
@@ -5782,13 +5780,13 @@
       <c r="U67" s="73"/>
       <c r="V67" s="52"/>
       <c r="W67" s="73"/>
-      <c r="X67" s="157"/>
+      <c r="X67" s="141"/>
       <c r="Y67" s="73"/>
       <c r="Z67" s="52"/>
       <c r="AA67" s="94"/>
       <c r="AB67" s="76"/>
     </row>
-    <row r="68" spans="1:28" s="46" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:28" s="46" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="135"/>
       <c r="B68" s="136"/>
       <c r="C68" s="137"/>
@@ -5812,20 +5810,20 @@
       <c r="U68" s="95"/>
       <c r="V68" s="96"/>
       <c r="W68" s="95"/>
-      <c r="X68" s="158"/>
+      <c r="X68" s="142"/>
       <c r="Y68" s="95"/>
       <c r="Z68" s="96"/>
       <c r="AA68" s="97"/>
       <c r="AB68" s="98"/>
     </row>
-    <row r="69" spans="1:28" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="156" t="s">
+    <row r="69" spans="1:28" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="150" t="s">
         <v>68</v>
       </c>
-      <c r="B69" s="156"/>
+      <c r="B69" s="150"/>
       <c r="C69" s="99">
         <f>SUM(C10:C68)</f>
-        <v>109.5</v>
+        <v>111</v>
       </c>
       <c r="D69" s="99">
         <f>SUM(D10:D68)</f>
@@ -5844,7 +5842,7 @@
       <c r="I69" s="101"/>
       <c r="J69" s="99">
         <f>SUM(C69:F69)</f>
-        <v>397.75</v>
+        <v>399.25</v>
       </c>
       <c r="K69" s="102"/>
       <c r="L69" s="102"/>
@@ -5868,14 +5866,14 @@
       </c>
       <c r="AB69" s="133"/>
     </row>
-    <row r="70" spans="1:28" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="151" t="s">
+    <row r="70" spans="1:28" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="145" t="s">
         <v>69</v>
       </c>
-      <c r="B70" s="151"/>
+      <c r="B70" s="145"/>
       <c r="C70" s="99">
         <f>135-C69</f>
-        <v>25.5</v>
+        <v>24</v>
       </c>
       <c r="D70" s="99">
         <f>135-D69</f>
@@ -5894,7 +5892,7 @@
       <c r="I70" s="99"/>
       <c r="J70" s="99">
         <f>SUM(C70:F70)</f>
-        <v>142.25</v>
+        <v>140.75</v>
       </c>
       <c r="K70" s="102"/>
       <c r="L70" s="102"/>
@@ -5915,11 +5913,11 @@
       <c r="AA70" s="102"/>
       <c r="AB70" s="102"/>
     </row>
-    <row r="71" spans="1:28" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="152" t="s">
+    <row r="71" spans="1:28" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="146" t="s">
         <v>70</v>
       </c>
-      <c r="B71" s="152"/>
+      <c r="B71" s="146"/>
       <c r="C71" s="99"/>
       <c r="D71" s="99"/>
       <c r="E71" s="99"/>
@@ -5950,11 +5948,11 @@
       <c r="AA71" s="102"/>
       <c r="AB71" s="102"/>
     </row>
-    <row r="72" spans="1:28" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="151" t="s">
+    <row r="72" spans="1:28" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="145" t="s">
         <v>71</v>
       </c>
-      <c r="B72" s="151"/>
+      <c r="B72" s="145"/>
       <c r="C72" s="99"/>
       <c r="D72" s="99"/>
       <c r="E72" s="103"/>
@@ -5967,7 +5965,7 @@
       </c>
       <c r="J72" s="99">
         <f>SUM(J10:J68)</f>
-        <v>397.75</v>
+        <v>399.25</v>
       </c>
       <c r="K72" s="102"/>
       <c r="L72" s="102"/>
@@ -5988,7 +5986,7 @@
       <c r="AA72" s="102"/>
       <c r="AB72" s="102"/>
     </row>
-    <row r="73" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="105"/>
       <c r="B73" s="105"/>
       <c r="C73" s="106"/>
@@ -6018,11 +6016,11 @@
       <c r="AA73" s="102"/>
       <c r="AB73" s="102"/>
     </row>
-    <row r="74" spans="1:28" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="152" t="s">
+    <row r="74" spans="1:28" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="146" t="s">
         <v>72</v>
       </c>
-      <c r="B74" s="152"/>
+      <c r="B74" s="146"/>
       <c r="C74" s="99">
         <f>135*4</f>
         <v>540</v>
@@ -6053,14 +6051,14 @@
       <c r="AA74" s="102"/>
       <c r="AB74" s="102"/>
     </row>
-    <row r="75" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A75" s="153" t="s">
+    <row r="75" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A75" s="147" t="s">
         <v>73</v>
       </c>
-      <c r="B75" s="153"/>
+      <c r="B75" s="147"/>
       <c r="C75" s="99">
         <f>C74-J72</f>
-        <v>142.25</v>
+        <v>140.75</v>
       </c>
       <c r="D75" s="106"/>
       <c r="E75" s="106"/>
@@ -6088,7 +6086,7 @@
       <c r="AA75" s="102"/>
       <c r="AB75" s="102"/>
     </row>
-    <row r="76" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="107"/>
       <c r="B76" s="105"/>
       <c r="C76" s="108"/>
@@ -6101,12 +6099,12 @@
       <c r="J76" s="110"/>
       <c r="AA76" s="102"/>
     </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:28" x14ac:dyDescent="0.2">
       <c r="D77" s="111"/>
       <c r="E77" s="111"/>
       <c r="F77" s="111"/>
     </row>
-    <row r="78" spans="1:28" s="113" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:28" s="113" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A78" s="112"/>
       <c r="C78" s="114"/>
       <c r="D78" s="114"/>
@@ -6121,7 +6119,7 @@
       <c r="Z78" s="117"/>
       <c r="AA78" s="118"/>
     </row>
-    <row r="79" spans="1:28" s="113" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:28" s="113" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="C79" s="114"/>
       <c r="D79" s="114"/>
       <c r="E79" s="114"/>
@@ -6135,7 +6133,7 @@
       <c r="Z79" s="117"/>
       <c r="AA79" s="118"/>
     </row>
-    <row r="80" spans="1:28" s="113" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:28" s="113" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="C80" s="114"/>
       <c r="D80" s="114"/>
       <c r="E80" s="114"/>
@@ -6151,14 +6149,11 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K6:R6"/>
     <mergeCell ref="S6:V6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
@@ -6168,11 +6163,14 @@
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="K7:Z7"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
   </mergeCells>
   <conditionalFormatting sqref="H19">
     <cfRule type="containsText" dxfId="44" priority="26" operator="containsText" text="En cours">
@@ -6367,12 +6365,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1025" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="119" t="s">
         <v>6</v>
       </c>
@@ -6380,7 +6378,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -6388,7 +6386,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -6408,7 +6406,7 @@
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1025" width="10.6640625" style="1"/>
   </cols>

</xml_diff>

<commit_message>
Ajout des taches devancer au sprint 1
</commit_message>
<xml_diff>
--- a/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire copy.xlsx
+++ b/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire copy.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Desktop/marque-sans-nom/Semainiers/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D2F4B0-F5D1-4144-B8B2-CFEF80DE356A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="18740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="23160" windowHeight="13080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="88">
   <si>
     <t>UQÀM - Hiver 2020</t>
   </si>
@@ -360,18 +354,21 @@
   <si>
     <t>Améliorer le visuel (messagerie) - REPOUSSÉ AU SPRINT 3</t>
   </si>
+  <si>
+    <t>Traduire les affichages</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_)_ ;_ * \(#,##0.00\)_ ;_ * \-??_)_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="0\ %"/>
     <numFmt numFmtId="166" formatCode="[$-C0C]dd/mmm"/>
     <numFmt numFmtId="167" formatCode="\\;;;"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -533,7 +530,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -603,6 +600,12 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="38">
     <border>
@@ -1095,7 +1098,7 @@
     <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="161">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1528,6 +1531,36 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1544,51 +1577,99 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="13" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Bad" xfId="10" builtinId="27"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Excel Built-in 60% - Accent4" xfId="7" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Excel Built-in Bad" xfId="6" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Excel Built-in Good" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Excel Built-in Neutral" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Excel Built-in Normal" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Excel Built-in 60% - Accent4" xfId="7"/>
+    <cellStyle name="Excel Built-in Bad" xfId="6"/>
+    <cellStyle name="Excel Built-in Good" xfId="4"/>
+    <cellStyle name="Excel Built-in Neutral" xfId="5"/>
+    <cellStyle name="Excel Built-in Normal" xfId="3"/>
     <cellStyle name="Good" xfId="8" builtinId="26"/>
     <cellStyle name="Neutral" xfId="9" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="67">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1683,6 +1764,177 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1949,43 +2201,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -2152,7 +2367,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2204,7 +2419,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2398,32 +2613,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AMK80"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="74.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="74.109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" style="2" customWidth="1"/>
-    <col min="4" max="5" width="8.1640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" style="3" customWidth="1"/>
     <col min="9" max="10" width="9.33203125" style="4" customWidth="1"/>
     <col min="11" max="13" width="8" style="1" customWidth="1"/>
     <col min="14" max="14" width="8" style="5" customWidth="1"/>
@@ -2439,23 +2654,23 @@
     <col min="29" max="1025" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="8" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="159" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="159"/>
+    <row r="1" spans="1:28" s="8" customFormat="1" ht="15.45" customHeight="1">
+      <c r="A1" s="145" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="145"/>
       <c r="C1" s="7"/>
-      <c r="D1" s="160" t="s">
+      <c r="D1" s="146" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="160"/>
-      <c r="F1" s="160"/>
-      <c r="G1" s="160"/>
-      <c r="H1" s="160"/>
-      <c r="I1" s="160"/>
-      <c r="J1" s="160"/>
-      <c r="K1" s="160"/>
-      <c r="L1" s="160"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
+      <c r="I1" s="146"/>
+      <c r="J1" s="146"/>
+      <c r="K1" s="146"/>
+      <c r="L1" s="146"/>
       <c r="N1" s="3"/>
       <c r="P1" s="9"/>
       <c r="Q1" s="8" t="s">
@@ -2466,21 +2681,21 @@
       <c r="Z1" s="3"/>
       <c r="AA1" s="10"/>
     </row>
-    <row r="2" spans="1:28" s="8" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="159" t="s">
+    <row r="2" spans="1:28" s="8" customFormat="1" ht="15.45" customHeight="1">
+      <c r="A2" s="145" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="159"/>
+      <c r="B2" s="145"/>
       <c r="C2" s="7"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
-      <c r="F2" s="159" t="s">
+      <c r="F2" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="159"/>
-      <c r="H2" s="159"/>
-      <c r="I2" s="159"/>
-      <c r="J2" s="159"/>
+      <c r="G2" s="145"/>
+      <c r="H2" s="145"/>
+      <c r="I2" s="145"/>
+      <c r="J2" s="145"/>
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
       <c r="N2" s="3"/>
@@ -2493,7 +2708,7 @@
       <c r="Z2" s="3"/>
       <c r="AA2" s="10"/>
     </row>
-    <row r="3" spans="1:28" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:28" s="8" customFormat="1" ht="15.6">
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -2511,7 +2726,7 @@
       <c r="Z3" s="3"/>
       <c r="AA3" s="10"/>
     </row>
-    <row r="4" spans="1:28" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:28" s="8" customFormat="1" ht="15.6">
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
@@ -2531,7 +2746,7 @@
       <c r="Z4" s="3"/>
       <c r="AA4" s="10"/>
     </row>
-    <row r="5" spans="1:28" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:28" s="8" customFormat="1" ht="15.6">
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
@@ -2555,7 +2770,7 @@
       </c>
       <c r="AA5" s="10"/>
     </row>
-    <row r="6" spans="1:28" s="8" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:28" s="8" customFormat="1" ht="16.2" customHeight="1">
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
@@ -2563,78 +2778,78 @@
       <c r="H6" s="3"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="151" t="s">
+      <c r="K6" s="147" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="151"/>
-      <c r="M6" s="151"/>
-      <c r="N6" s="151"/>
-      <c r="O6" s="151"/>
-      <c r="P6" s="151"/>
-      <c r="Q6" s="151"/>
-      <c r="R6" s="151"/>
-      <c r="S6" s="151" t="s">
+      <c r="L6" s="147"/>
+      <c r="M6" s="147"/>
+      <c r="N6" s="147"/>
+      <c r="O6" s="147"/>
+      <c r="P6" s="147"/>
+      <c r="Q6" s="147"/>
+      <c r="R6" s="147"/>
+      <c r="S6" s="147" t="s">
         <v>10</v>
       </c>
-      <c r="T6" s="151"/>
-      <c r="U6" s="151"/>
-      <c r="V6" s="151"/>
+      <c r="T6" s="147"/>
+      <c r="U6" s="147"/>
+      <c r="V6" s="147"/>
       <c r="Z6" s="17"/>
       <c r="AA6" s="10"/>
     </row>
-    <row r="7" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="152" t="s">
+    <row r="7" spans="1:28" ht="19.5" customHeight="1">
+      <c r="A7" s="148" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="153" t="s">
+      <c r="B7" s="149" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="154" t="s">
+      <c r="C7" s="150" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="154"/>
-      <c r="E7" s="154"/>
-      <c r="F7" s="154"/>
-      <c r="G7" s="155" t="s">
+      <c r="D7" s="150"/>
+      <c r="E7" s="150"/>
+      <c r="F7" s="150"/>
+      <c r="G7" s="151" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="156" t="s">
+      <c r="H7" s="152" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="157" t="s">
+      <c r="I7" s="153" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="157" t="s">
+      <c r="J7" s="153" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="158" t="s">
+      <c r="K7" s="154" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="158"/>
-      <c r="M7" s="158"/>
-      <c r="N7" s="158"/>
-      <c r="O7" s="158"/>
-      <c r="P7" s="158"/>
-      <c r="Q7" s="158"/>
-      <c r="R7" s="158"/>
-      <c r="S7" s="158"/>
-      <c r="T7" s="158"/>
-      <c r="U7" s="158"/>
-      <c r="V7" s="158"/>
-      <c r="W7" s="158"/>
-      <c r="X7" s="158"/>
-      <c r="Y7" s="158"/>
-      <c r="Z7" s="158"/>
-      <c r="AA7" s="148" t="s">
+      <c r="L7" s="154"/>
+      <c r="M7" s="154"/>
+      <c r="N7" s="154"/>
+      <c r="O7" s="154"/>
+      <c r="P7" s="154"/>
+      <c r="Q7" s="154"/>
+      <c r="R7" s="154"/>
+      <c r="S7" s="154"/>
+      <c r="T7" s="154"/>
+      <c r="U7" s="154"/>
+      <c r="V7" s="154"/>
+      <c r="W7" s="154"/>
+      <c r="X7" s="154"/>
+      <c r="Y7" s="154"/>
+      <c r="Z7" s="154"/>
+      <c r="AA7" s="158" t="s">
         <v>19</v>
       </c>
-      <c r="AB7" s="149" t="s">
+      <c r="AB7" s="159" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="152"/>
-      <c r="B8" s="153"/>
+    <row r="8" spans="1:28" ht="18.75" customHeight="1">
+      <c r="A8" s="148"/>
+      <c r="B8" s="149"/>
       <c r="C8" s="20" t="s">
         <v>21</v>
       </c>
@@ -2647,10 +2862,10 @@
       <c r="F8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="155"/>
-      <c r="H8" s="156"/>
-      <c r="I8" s="157"/>
-      <c r="J8" s="157"/>
+      <c r="G8" s="151"/>
+      <c r="H8" s="152"/>
+      <c r="I8" s="153"/>
+      <c r="J8" s="153"/>
       <c r="K8" s="21">
         <v>43838</v>
       </c>
@@ -2714,10 +2929,10 @@
         <f t="shared" si="0"/>
         <v>43943</v>
       </c>
-      <c r="AA8" s="148"/>
-      <c r="AB8" s="149"/>
-    </row>
-    <row r="9" spans="1:28" ht="19" x14ac:dyDescent="0.2">
+      <c r="AA8" s="158"/>
+      <c r="AB8" s="159"/>
+    </row>
+    <row r="9" spans="1:28" ht="18">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>25</v>
@@ -2749,7 +2964,7 @@
       <c r="AA9" s="33"/>
       <c r="AB9" s="34"/>
     </row>
-    <row r="10" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A10" s="35">
         <v>1</v>
       </c>
@@ -2804,7 +3019,7 @@
       </c>
       <c r="AB10" s="45"/>
     </row>
-    <row r="11" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A11" s="35">
         <v>2</v>
       </c>
@@ -2859,7 +3074,7 @@
       </c>
       <c r="AB11" s="48"/>
     </row>
-    <row r="12" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A12" s="35">
         <v>3</v>
       </c>
@@ -2913,7 +3128,7 @@
       </c>
       <c r="AB12" s="49"/>
     </row>
-    <row r="13" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A13" s="35">
         <v>4</v>
       </c>
@@ -2968,7 +3183,7 @@
       </c>
       <c r="AB13" s="48"/>
     </row>
-    <row r="14" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A14" s="35">
         <v>5</v>
       </c>
@@ -3023,7 +3238,7 @@
       </c>
       <c r="AB14" s="48"/>
     </row>
-    <row r="15" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A15" s="35">
         <v>6</v>
       </c>
@@ -3078,7 +3293,7 @@
       </c>
       <c r="AB15" s="48"/>
     </row>
-    <row r="16" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A16" s="35">
         <v>7</v>
       </c>
@@ -3133,7 +3348,7 @@
       </c>
       <c r="AB16" s="48"/>
     </row>
-    <row r="17" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A17" s="35">
         <v>8</v>
       </c>
@@ -3188,7 +3403,7 @@
       </c>
       <c r="AB17" s="48"/>
     </row>
-    <row r="18" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A18" s="35">
         <v>9</v>
       </c>
@@ -3243,7 +3458,7 @@
       </c>
       <c r="AB18" s="48"/>
     </row>
-    <row r="19" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A19" s="35">
         <v>10</v>
       </c>
@@ -3298,7 +3513,7 @@
       </c>
       <c r="AB19" s="48"/>
     </row>
-    <row r="20" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A20" s="35">
         <v>11</v>
       </c>
@@ -3353,7 +3568,7 @@
       </c>
       <c r="AB20" s="48"/>
     </row>
-    <row r="21" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" s="46" customFormat="1">
       <c r="A21" s="35">
         <v>12</v>
       </c>
@@ -3408,7 +3623,7 @@
       </c>
       <c r="AB21" s="48"/>
     </row>
-    <row r="22" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A22" s="35">
         <v>13</v>
       </c>
@@ -3463,7 +3678,7 @@
       </c>
       <c r="AB22" s="48"/>
     </row>
-    <row r="23" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A23" s="35">
         <v>14</v>
       </c>
@@ -3518,7 +3733,7 @@
       </c>
       <c r="AB23" s="48"/>
     </row>
-    <row r="24" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A24" s="35">
         <v>15</v>
       </c>
@@ -3573,7 +3788,7 @@
       </c>
       <c r="AB24" s="48"/>
     </row>
-    <row r="25" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A25" s="35">
         <v>16</v>
       </c>
@@ -3628,7 +3843,7 @@
       </c>
       <c r="AB25" s="48"/>
     </row>
-    <row r="26" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A26" s="35">
         <v>17</v>
       </c>
@@ -3683,7 +3898,7 @@
       </c>
       <c r="AB26" s="76"/>
     </row>
-    <row r="27" spans="1:28" s="79" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" s="79" customFormat="1" ht="15.6">
       <c r="A27" s="35">
         <v>18</v>
       </c>
@@ -3738,7 +3953,7 @@
       </c>
       <c r="AB27" s="48"/>
     </row>
-    <row r="28" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A28" s="35">
         <v>19</v>
       </c>
@@ -3793,7 +4008,7 @@
       </c>
       <c r="AB28" s="48"/>
     </row>
-    <row r="29" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A29" s="35">
         <v>20</v>
       </c>
@@ -3848,7 +4063,7 @@
       </c>
       <c r="AB29" s="48"/>
     </row>
-    <row r="30" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A30" s="35">
         <v>21</v>
       </c>
@@ -3903,7 +4118,7 @@
       </c>
       <c r="AB30" s="48"/>
     </row>
-    <row r="31" spans="1:28" s="79" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" s="79" customFormat="1" ht="15.6">
       <c r="A31" s="35">
         <v>22</v>
       </c>
@@ -3958,7 +4173,7 @@
       </c>
       <c r="AB31" s="48"/>
     </row>
-    <row r="32" spans="1:28" s="79" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" s="79" customFormat="1" ht="15.6">
       <c r="A32" s="35">
         <v>23</v>
       </c>
@@ -4013,7 +4228,7 @@
       </c>
       <c r="AB32" s="48"/>
     </row>
-    <row r="33" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A33" s="35">
         <v>24</v>
       </c>
@@ -4068,7 +4283,7 @@
       </c>
       <c r="AB33" s="48"/>
     </row>
-    <row r="34" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A34" s="35">
         <v>25</v>
       </c>
@@ -4123,7 +4338,7 @@
       </c>
       <c r="AB34" s="48"/>
     </row>
-    <row r="35" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A35" s="35">
         <v>27</v>
       </c>
@@ -4176,7 +4391,7 @@
       </c>
       <c r="AB35" s="48"/>
     </row>
-    <row r="36" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A36" s="35">
         <v>28</v>
       </c>
@@ -4229,7 +4444,7 @@
       </c>
       <c r="AB36" s="48"/>
     </row>
-    <row r="37" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A37" s="35">
         <v>29</v>
       </c>
@@ -4282,7 +4497,7 @@
       </c>
       <c r="AB37" s="48"/>
     </row>
-    <row r="38" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A38" s="35">
         <v>30</v>
       </c>
@@ -4335,7 +4550,7 @@
       </c>
       <c r="AB38" s="48"/>
     </row>
-    <row r="39" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A39" s="35">
         <v>31</v>
       </c>
@@ -4388,7 +4603,7 @@
       </c>
       <c r="AB39" s="48"/>
     </row>
-    <row r="40" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A40" s="35">
         <v>32</v>
       </c>
@@ -4441,7 +4656,7 @@
       </c>
       <c r="AB40" s="48"/>
     </row>
-    <row r="41" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A41" s="35">
         <v>33</v>
       </c>
@@ -4452,7 +4667,7 @@
         <v>2</v>
       </c>
       <c r="D41" s="37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E41" s="37">
         <v>2</v>
@@ -4472,7 +4687,7 @@
       </c>
       <c r="J41" s="40">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K41" s="73"/>
       <c r="L41" s="73"/>
@@ -4492,11 +4707,11 @@
       <c r="Z41" s="52"/>
       <c r="AA41" s="44">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB41" s="48"/>
     </row>
-    <row r="42" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:28" s="46" customFormat="1">
       <c r="A42" s="35">
         <v>34</v>
       </c>
@@ -4549,7 +4764,7 @@
       </c>
       <c r="AB42" s="48"/>
     </row>
-    <row r="43" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A43" s="35">
         <v>35</v>
       </c>
@@ -4604,7 +4819,7 @@
       </c>
       <c r="AB43" s="48"/>
     </row>
-    <row r="44" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:28" s="46" customFormat="1">
       <c r="A44" s="35">
         <v>36</v>
       </c>
@@ -4659,7 +4874,7 @@
       </c>
       <c r="AB44" s="48"/>
     </row>
-    <row r="45" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A45" s="35">
         <v>37</v>
       </c>
@@ -4712,7 +4927,7 @@
       </c>
       <c r="AB45" s="48"/>
     </row>
-    <row r="46" spans="1:28" s="86" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:28" s="86" customFormat="1">
       <c r="A46" s="35">
         <v>39</v>
       </c>
@@ -4764,7 +4979,7 @@
       <c r="AA46" s="44"/>
       <c r="AB46" s="48"/>
     </row>
-    <row r="47" spans="1:28" s="86" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:28" s="86" customFormat="1" ht="15.6">
       <c r="A47" s="35">
         <v>40</v>
       </c>
@@ -4816,7 +5031,7 @@
       <c r="AA47" s="44"/>
       <c r="AB47" s="48"/>
     </row>
-    <row r="48" spans="1:28" s="46" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:28" s="46" customFormat="1" ht="18">
       <c r="A48" s="87"/>
       <c r="B48" s="24" t="s">
         <v>64</v>
@@ -4848,7 +5063,7 @@
       <c r="AA48" s="90"/>
       <c r="AB48" s="91"/>
     </row>
-    <row r="49" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A49" s="35">
         <v>1</v>
       </c>
@@ -4903,7 +5118,7 @@
       </c>
       <c r="AB49" s="48"/>
     </row>
-    <row r="50" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A50" s="35">
         <v>2</v>
       </c>
@@ -4956,7 +5171,7 @@
       </c>
       <c r="AB50" s="48"/>
     </row>
-    <row r="51" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A51" s="35">
         <v>3</v>
       </c>
@@ -5006,7 +5221,7 @@
       <c r="AA51" s="94"/>
       <c r="AB51" s="76"/>
     </row>
-    <row r="52" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A52" s="35">
         <v>4</v>
       </c>
@@ -5058,7 +5273,7 @@
       <c r="AA52" s="94"/>
       <c r="AB52" s="76"/>
     </row>
-    <row r="53" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A53" s="143">
         <v>5</v>
       </c>
@@ -5110,7 +5325,7 @@
       <c r="AA53" s="94"/>
       <c r="AB53" s="76"/>
     </row>
-    <row r="54" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A54" s="35">
         <v>6</v>
       </c>
@@ -5162,7 +5377,7 @@
       <c r="AA54" s="94"/>
       <c r="AB54" s="76"/>
     </row>
-    <row r="55" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A55" s="35">
         <v>7</v>
       </c>
@@ -5214,7 +5429,7 @@
       <c r="AA55" s="94"/>
       <c r="AB55" s="76"/>
     </row>
-    <row r="56" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A56" s="35">
         <v>8</v>
       </c>
@@ -5266,7 +5481,7 @@
       <c r="AA56" s="94"/>
       <c r="AB56" s="76"/>
     </row>
-    <row r="57" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A57" s="35">
         <v>9</v>
       </c>
@@ -5318,7 +5533,7 @@
       <c r="AA57" s="94"/>
       <c r="AB57" s="76"/>
     </row>
-    <row r="58" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A58" s="35">
         <v>10</v>
       </c>
@@ -5370,7 +5585,7 @@
       <c r="AA58" s="94"/>
       <c r="AB58" s="76"/>
     </row>
-    <row r="59" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A59" s="35">
         <v>11</v>
       </c>
@@ -5422,7 +5637,7 @@
       <c r="AA59" s="94"/>
       <c r="AB59" s="76"/>
     </row>
-    <row r="60" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A60" s="35">
         <v>12</v>
       </c>
@@ -5474,7 +5689,7 @@
       <c r="AA60" s="94"/>
       <c r="AB60" s="76"/>
     </row>
-    <row r="61" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A61" s="35">
         <v>13</v>
       </c>
@@ -5526,7 +5741,7 @@
       <c r="AA61" s="94"/>
       <c r="AB61" s="76"/>
     </row>
-    <row r="62" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A62" s="35">
         <v>14</v>
       </c>
@@ -5578,7 +5793,7 @@
       <c r="AA62" s="94"/>
       <c r="AB62" s="76"/>
     </row>
-    <row r="63" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A63" s="35">
         <v>15</v>
       </c>
@@ -5630,7 +5845,7 @@
       <c r="AA63" s="94"/>
       <c r="AB63" s="76"/>
     </row>
-    <row r="64" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A64" s="143">
         <v>17</v>
       </c>
@@ -5677,7 +5892,7 @@
       <c r="AA64" s="94"/>
       <c r="AB64" s="76"/>
     </row>
-    <row r="65" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A65" s="35">
         <v>18</v>
       </c>
@@ -5688,7 +5903,7 @@
         <v>1.5</v>
       </c>
       <c r="D65" s="37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E65" s="37">
         <v>1.5</v>
@@ -5704,8 +5919,8 @@
         <v>3</v>
       </c>
       <c r="J65" s="40">
-        <f t="shared" ref="J65" si="5">SUM(C65:F65)</f>
-        <v>3</v>
+        <f t="shared" ref="J65:J66" si="5">SUM(C65:F65)</f>
+        <v>3.5</v>
       </c>
       <c r="K65" s="73"/>
       <c r="L65" s="73"/>
@@ -5726,17 +5941,36 @@
       <c r="AA65" s="94"/>
       <c r="AB65" s="76"/>
     </row>
-    <row r="66" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A66" s="35"/>
-      <c r="B66" s="69"/>
-      <c r="C66" s="37"/>
-      <c r="D66" s="37"/>
-      <c r="E66" s="37"/>
-      <c r="F66" s="37"/>
+    <row r="66" spans="1:28" s="46" customFormat="1" ht="15.6">
+      <c r="A66" s="35">
+        <v>19</v>
+      </c>
+      <c r="B66" s="69" t="s">
+        <v>87</v>
+      </c>
+      <c r="C66" s="161">
+        <v>0</v>
+      </c>
+      <c r="D66" s="161">
+        <v>1</v>
+      </c>
+      <c r="E66" s="37">
+        <v>0</v>
+      </c>
+      <c r="F66" s="37">
+        <v>0</v>
+      </c>
       <c r="G66" s="71"/>
-      <c r="H66" s="39"/>
-      <c r="I66" s="40"/>
-      <c r="J66" s="40"/>
+      <c r="H66" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="I66" s="40">
+        <v>5</v>
+      </c>
+      <c r="J66" s="40">
+        <f t="shared" ref="J66" si="6">SUM(C66:F66)</f>
+        <v>1</v>
+      </c>
       <c r="K66" s="73"/>
       <c r="L66" s="73"/>
       <c r="M66" s="73"/>
@@ -5750,13 +5984,13 @@
       <c r="U66" s="73"/>
       <c r="V66" s="52"/>
       <c r="W66" s="73"/>
-      <c r="X66" s="141"/>
+      <c r="X66" s="128"/>
       <c r="Y66" s="73"/>
       <c r="Z66" s="52"/>
       <c r="AA66" s="94"/>
       <c r="AB66" s="76"/>
     </row>
-    <row r="67" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:28" s="46" customFormat="1" ht="15.6">
       <c r="A67" s="35"/>
       <c r="B67" s="69"/>
       <c r="C67" s="37"/>
@@ -5786,7 +6020,7 @@
       <c r="AA67" s="94"/>
       <c r="AB67" s="76"/>
     </row>
-    <row r="68" spans="1:28" s="46" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" s="46" customFormat="1" ht="16.2" thickBot="1">
       <c r="A68" s="135"/>
       <c r="B68" s="136"/>
       <c r="C68" s="137"/>
@@ -5816,18 +6050,18 @@
       <c r="AA68" s="97"/>
       <c r="AB68" s="98"/>
     </row>
-    <row r="69" spans="1:28" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="150" t="s">
+    <row r="69" spans="1:28" ht="16.5" customHeight="1" thickBot="1">
+      <c r="A69" s="160" t="s">
         <v>68</v>
       </c>
-      <c r="B69" s="150"/>
+      <c r="B69" s="160"/>
       <c r="C69" s="99">
         <f>SUM(C10:C68)</f>
         <v>111</v>
       </c>
       <c r="D69" s="99">
         <f>SUM(D10:D68)</f>
-        <v>88</v>
+        <v>90.5</v>
       </c>
       <c r="E69" s="99">
         <f>SUM(E10:E68)</f>
@@ -5842,7 +6076,7 @@
       <c r="I69" s="101"/>
       <c r="J69" s="99">
         <f>SUM(C69:F69)</f>
-        <v>399.25</v>
+        <v>401.75</v>
       </c>
       <c r="K69" s="102"/>
       <c r="L69" s="102"/>
@@ -5862,22 +6096,22 @@
       <c r="Z69" s="102"/>
       <c r="AA69" s="132">
         <f>SUM(AA10:AA68)</f>
-        <v>0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="AB69" s="133"/>
     </row>
-    <row r="70" spans="1:28" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="145" t="s">
+    <row r="70" spans="1:28" ht="16.95" customHeight="1" thickBot="1">
+      <c r="A70" s="155" t="s">
         <v>69</v>
       </c>
-      <c r="B70" s="145"/>
+      <c r="B70" s="155"/>
       <c r="C70" s="99">
         <f>135-C69</f>
         <v>24</v>
       </c>
       <c r="D70" s="99">
         <f>135-D69</f>
-        <v>47</v>
+        <v>44.5</v>
       </c>
       <c r="E70" s="99">
         <f>135-E69</f>
@@ -5892,7 +6126,7 @@
       <c r="I70" s="99"/>
       <c r="J70" s="99">
         <f>SUM(C70:F70)</f>
-        <v>140.75</v>
+        <v>138.25</v>
       </c>
       <c r="K70" s="102"/>
       <c r="L70" s="102"/>
@@ -5913,11 +6147,11 @@
       <c r="AA70" s="102"/>
       <c r="AB70" s="102"/>
     </row>
-    <row r="71" spans="1:28" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="146" t="s">
+    <row r="71" spans="1:28" ht="16.95" customHeight="1">
+      <c r="A71" s="156" t="s">
         <v>70</v>
       </c>
-      <c r="B71" s="146"/>
+      <c r="B71" s="156"/>
       <c r="C71" s="99"/>
       <c r="D71" s="99"/>
       <c r="E71" s="99"/>
@@ -5948,11 +6182,11 @@
       <c r="AA71" s="102"/>
       <c r="AB71" s="102"/>
     </row>
-    <row r="72" spans="1:28" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="145" t="s">
+    <row r="72" spans="1:28" ht="16.95" customHeight="1">
+      <c r="A72" s="155" t="s">
         <v>71</v>
       </c>
-      <c r="B72" s="145"/>
+      <c r="B72" s="155"/>
       <c r="C72" s="99"/>
       <c r="D72" s="99"/>
       <c r="E72" s="103"/>
@@ -5961,11 +6195,11 @@
       <c r="H72" s="99"/>
       <c r="I72" s="104">
         <f>SUM(I10:I68)</f>
-        <v>399.25</v>
+        <v>404.25</v>
       </c>
       <c r="J72" s="99">
         <f>SUM(J10:J68)</f>
-        <v>399.25</v>
+        <v>401.75</v>
       </c>
       <c r="K72" s="102"/>
       <c r="L72" s="102"/>
@@ -5986,7 +6220,7 @@
       <c r="AA72" s="102"/>
       <c r="AB72" s="102"/>
     </row>
-    <row r="73" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:28" ht="15.6">
       <c r="A73" s="105"/>
       <c r="B73" s="105"/>
       <c r="C73" s="106"/>
@@ -6016,11 +6250,11 @@
       <c r="AA73" s="102"/>
       <c r="AB73" s="102"/>
     </row>
-    <row r="74" spans="1:28" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="146" t="s">
+    <row r="74" spans="1:28" ht="16.2" customHeight="1">
+      <c r="A74" s="156" t="s">
         <v>72</v>
       </c>
-      <c r="B74" s="146"/>
+      <c r="B74" s="156"/>
       <c r="C74" s="99">
         <f>135*4</f>
         <v>540</v>
@@ -6051,14 +6285,14 @@
       <c r="AA74" s="102"/>
       <c r="AB74" s="102"/>
     </row>
-    <row r="75" spans="1:28" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75" s="147" t="s">
+    <row r="75" spans="1:28" ht="15.6">
+      <c r="A75" s="157" t="s">
         <v>73</v>
       </c>
-      <c r="B75" s="147"/>
+      <c r="B75" s="157"/>
       <c r="C75" s="99">
         <f>C74-J72</f>
-        <v>140.75</v>
+        <v>138.25</v>
       </c>
       <c r="D75" s="106"/>
       <c r="E75" s="106"/>
@@ -6086,7 +6320,7 @@
       <c r="AA75" s="102"/>
       <c r="AB75" s="102"/>
     </row>
-    <row r="76" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:28" ht="15.6">
       <c r="A76" s="107"/>
       <c r="B76" s="105"/>
       <c r="C76" s="108"/>
@@ -6099,12 +6333,12 @@
       <c r="J76" s="110"/>
       <c r="AA76" s="102"/>
     </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:28">
       <c r="D77" s="111"/>
       <c r="E77" s="111"/>
       <c r="F77" s="111"/>
     </row>
-    <row r="78" spans="1:28" s="113" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:28" s="113" customFormat="1" ht="13.8">
       <c r="A78" s="112"/>
       <c r="C78" s="114"/>
       <c r="D78" s="114"/>
@@ -6119,7 +6353,7 @@
       <c r="Z78" s="117"/>
       <c r="AA78" s="118"/>
     </row>
-    <row r="79" spans="1:28" s="113" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:28" s="113" customFormat="1" ht="13.8">
       <c r="C79" s="114"/>
       <c r="D79" s="114"/>
       <c r="E79" s="114"/>
@@ -6133,7 +6367,7 @@
       <c r="Z79" s="117"/>
       <c r="AA79" s="118"/>
     </row>
-    <row r="80" spans="1:28" s="113" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:28" s="113" customFormat="1" ht="13.8">
       <c r="C80" s="114"/>
       <c r="D80" s="114"/>
       <c r="E80" s="114"/>
@@ -6149,11 +6383,14 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
     <mergeCell ref="S6:V6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
@@ -6163,190 +6400,214 @@
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="K7:Z7"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K6:R6"/>
   </mergeCells>
   <conditionalFormatting sqref="H19">
-    <cfRule type="containsText" dxfId="44" priority="26" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="66" priority="33" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",H19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H45 H49 H47">
-    <cfRule type="containsText" dxfId="43" priority="27" operator="containsText" text="En attente">
+    <cfRule type="containsText" dxfId="65" priority="34" operator="containsText" text="En attente">
       <formula>NOT(ISERROR(SEARCH("En attente",H9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="28" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="64" priority="35" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",H9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="29" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="63" priority="36" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",H9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:F45 C47:F47 C56:F64 C49:F54 C66:F68">
-    <cfRule type="cellIs" dxfId="40" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="37" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="31">
+    <cfRule type="expression" dxfId="13" priority="38">
       <formula>$H9="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:F45 C47:F47 C56:F64 C49:F54 C66:F68">
-    <cfRule type="expression" dxfId="38" priority="32">
+    <cfRule type="expression" dxfId="12" priority="39">
       <formula>$H9="En cours"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="33">
+    <cfRule type="expression" dxfId="11" priority="40">
       <formula>$H9="En attente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="containsText" dxfId="36" priority="34" operator="containsText" text="En attente">
+    <cfRule type="containsText" dxfId="62" priority="41" operator="containsText" text="En attente">
       <formula>NOT(ISERROR(SEARCH("En attente",H48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="35" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="61" priority="42" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",H48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="36" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="60" priority="43" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",H48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:F48">
-    <cfRule type="cellIs" dxfId="33" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="44" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="38">
+    <cfRule type="expression" dxfId="58" priority="45">
       <formula>$H48="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:F48">
-    <cfRule type="expression" dxfId="31" priority="39">
+    <cfRule type="expression" dxfId="57" priority="46">
       <formula>$H48="En cours"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="40">
+    <cfRule type="expression" dxfId="56" priority="47">
       <formula>$H48="En attente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H50:H54">
-    <cfRule type="containsText" dxfId="29" priority="41" operator="containsText" text="En attente">
+    <cfRule type="containsText" dxfId="55" priority="48" operator="containsText" text="En attente">
       <formula>NOT(ISERROR(SEARCH("En attente",H50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="42" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="54" priority="49" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",H50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="43" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="53" priority="50" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",H50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46">
-    <cfRule type="containsText" dxfId="26" priority="48" operator="containsText" text="En attente">
+    <cfRule type="containsText" dxfId="52" priority="55" operator="containsText" text="En attente">
       <formula>NOT(ISERROR(SEARCH("En attente",H46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="49" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="51" priority="56" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",H46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="50" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="50" priority="57" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",H46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:F46">
-    <cfRule type="cellIs" dxfId="23" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="58" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="52">
+    <cfRule type="expression" dxfId="48" priority="59">
       <formula>$H46="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:F46">
-    <cfRule type="expression" dxfId="21" priority="53">
+    <cfRule type="expression" dxfId="47" priority="60">
       <formula>$H46="En cours"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="54">
+    <cfRule type="expression" dxfId="46" priority="61">
       <formula>$H46="En attente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="containsText" dxfId="19" priority="18" operator="containsText" text="En attente">
+    <cfRule type="containsText" dxfId="45" priority="25" operator="containsText" text="En attente">
       <formula>NOT(ISERROR(SEARCH("En attente",H55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="44" priority="26" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",H55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="20" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="43" priority="27" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",H55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:F55">
-    <cfRule type="cellIs" dxfId="16" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="28" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="22">
+    <cfRule type="expression" dxfId="41" priority="29">
       <formula>$H55="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:F55">
-    <cfRule type="expression" dxfId="14" priority="23">
+    <cfRule type="expression" dxfId="40" priority="30">
       <formula>$H55="En cours"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="24">
+    <cfRule type="expression" dxfId="39" priority="31">
       <formula>$H55="En attente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H56:H61">
-    <cfRule type="containsText" dxfId="12" priority="11" operator="containsText" text="En attente">
+    <cfRule type="containsText" dxfId="38" priority="18" operator="containsText" text="En attente">
       <formula>NOT(ISERROR(SEARCH("En attente",H56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="37" priority="19" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",H56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="13" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="36" priority="20" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",H56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H62:H64 H66:H68">
-    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="En attente">
+    <cfRule type="containsText" dxfId="10" priority="15" operator="containsText" text="En attente">
       <formula>NOT(ISERROR(SEARCH("En attente",H62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="9" priority="16" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",H62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="8" priority="17" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",H62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65:F65">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="34" priority="12">
       <formula>$H65="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65:F65">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="33" priority="13">
       <formula>$H65="En cours"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="7">
+    <cfRule type="expression" dxfId="32" priority="14">
       <formula>$H65="En attente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H65">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="En attente">
+    <cfRule type="containsText" dxfId="31" priority="8" operator="containsText" text="En attente">
       <formula>NOT(ISERROR(SEARCH("En attente",H65)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="30" priority="9" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",H65)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="29" priority="10" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",H65)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C66:F66">
+    <cfRule type="cellIs" dxfId="28" priority="6" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="7">
+      <formula>$H66="Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C66:F66">
+    <cfRule type="expression" dxfId="24" priority="4">
+      <formula>$H66="En cours"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="5">
+      <formula>$H66="En attente"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H66">
+    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="En attente">
+      <formula>NOT(ISERROR(SEARCH("En attente",H66)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="2" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",H66)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="3" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",H66)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H9:H68" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H9:H68">
       <formula1>"En attente,En cours,Terminé"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6358,19 +6619,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMK3"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1025" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="119" t="s">
         <v>6</v>
       </c>
@@ -6378,7 +6639,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -6386,7 +6647,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -6401,12 +6662,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMK1"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1025" width="10.6640625" style="1"/>
   </cols>

</xml_diff>